<commit_message>
more catching of incomplete format of excel file
</commit_message>
<xml_diff>
--- a/spec/files/small_list.xlsx
+++ b/spec/files/small_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="0" windowWidth="25600" windowHeight="27520" activeTab="1"/>
+    <workbookView xWindow="25600" yWindow="0" windowWidth="25600" windowHeight="27520" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -1487,8 +1487,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1233">
+  <cellStyleXfs count="1235">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2772,7 +2774,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1233">
+  <cellStyles count="1235">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3389,6 +3391,7 @@
     <cellStyle name="Followed Hyperlink" xfId="1228" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1230" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1234" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4005,6 +4008,7 @@
     <cellStyle name="Hyperlink" xfId="1227" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1229" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1233" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4340,7 +4344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B15" sqref="B15:D15"/>
     </sheetView>
   </sheetViews>
@@ -4492,9 +4496,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+      <selection pane="bottomLeft" activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5097,7 +5101,9 @@
       <c r="K21" s="3">
         <v>4</v>
       </c>
-      <c r="L21" s="3"/>
+      <c r="L21" s="3">
+        <v>0</v>
+      </c>
       <c r="M21" s="3">
         <f>(K21-J21)/6</f>
         <v>1.3333333333333333</v>
@@ -5134,7 +5140,9 @@
       <c r="K22" s="3">
         <v>-4</v>
       </c>
-      <c r="L22" s="3"/>
+      <c r="L22" s="3">
+        <v>0</v>
+      </c>
       <c r="M22" s="3">
         <f>(K22-J22)/6</f>
         <v>-1.3333333333333333</v>
@@ -5494,6 +5502,10 @@
       </c>
       <c r="L36" s="20">
         <v>25</v>
+      </c>
+      <c r="M36" s="3">
+        <f>(K36-J36)/6</f>
+        <v>8.3333333333333339</v>
       </c>
       <c r="N36" s="1" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
multiple variable name check
</commit_message>
<xml_diff>
--- a/spec/files/small_list.xlsx
+++ b/spec/files/small_list.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1843" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1812" uniqueCount="456">
   <si>
     <t>type</t>
   </si>
@@ -1387,6 +1387,12 @@
   </si>
   <si>
     <t>../../spec/files/small_seed.osm</t>
+  </si>
+  <si>
+    <t>Roof R Value</t>
+  </si>
+  <si>
+    <t>Wall R Value</t>
   </si>
 </sst>
 </file>
@@ -4494,11 +4500,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V42"/>
+  <dimension ref="A1:V36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M36" sqref="M36"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5199,7 +5205,7 @@
         <v>27</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>271</v>
+        <v>455</v>
       </c>
       <c r="D25" s="20" t="s">
         <v>272</v>
@@ -5326,7 +5332,7 @@
         <v>27</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>271</v>
+        <v>454</v>
       </c>
       <c r="D30" s="20" t="s">
         <v>272</v>
@@ -5433,10 +5439,10 @@
         <v>1</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>81</v>
+        <v>341</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>81</v>
+        <v>342</v>
       </c>
       <c r="D34" s="20" t="s">
         <v>80</v>
@@ -5478,10 +5484,10 @@
         <v>27</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>82</v>
+        <v>344</v>
       </c>
       <c r="E36" s="20" t="s">
         <v>15</v>
@@ -5491,175 +5497,23 @@
       </c>
       <c r="G36" s="20"/>
       <c r="H36" s="20">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I36" s="20"/>
       <c r="J36">
         <v>0</v>
       </c>
       <c r="K36">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="L36" s="20">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="M36" s="3">
         <f>(K36-J36)/6</f>
-        <v>8.3333333333333339</v>
+        <v>15</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" customFormat="1" ht="15">
-      <c r="A37" s="20"/>
-      <c r="B37" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C37" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="D37" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="E37" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F37" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20">
-        <v>0</v>
-      </c>
-      <c r="I37" s="20"/>
-    </row>
-    <row r="38" spans="1:14" customFormat="1" ht="15">
-      <c r="A38" s="20"/>
-      <c r="B38" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C38" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="D38" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="E38" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F38" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20">
-        <v>0</v>
-      </c>
-      <c r="I38" s="20"/>
-    </row>
-    <row r="39" spans="1:14" customFormat="1" ht="15">
-      <c r="A39" s="20"/>
-      <c r="B39" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C39" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D39" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="E39" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F39" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20">
-        <v>1</v>
-      </c>
-      <c r="I39" s="20"/>
-    </row>
-    <row r="40" spans="1:14" customFormat="1" ht="15">
-      <c r="A40" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="B40" s="20" t="s">
-        <v>341</v>
-      </c>
-      <c r="C40" s="20" t="s">
-        <v>342</v>
-      </c>
-      <c r="D40" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="20"/>
-    </row>
-    <row r="41" spans="1:14" customFormat="1" ht="15">
-      <c r="A41" s="20"/>
-      <c r="B41" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C41" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D41" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="E41" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F41" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="I41" s="20" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" customFormat="1" ht="15">
-      <c r="A42" s="20"/>
-      <c r="B42" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C42" s="20" t="s">
-        <v>343</v>
-      </c>
-      <c r="D42" s="20" t="s">
-        <v>344</v>
-      </c>
-      <c r="E42" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="F42" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20">
-        <v>0</v>
-      </c>
-      <c r="I42" s="20"/>
-      <c r="J42">
-        <v>0</v>
-      </c>
-      <c r="K42">
-        <v>90</v>
-      </c>
-      <c r="L42" s="20">
-        <v>20</v>
-      </c>
-      <c r="M42" s="3">
-        <f>(K42-J42)/6</f>
-        <v>15</v>
-      </c>
-      <c r="N42" s="1" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
catch when min is greater than max
</commit_message>
<xml_diff>
--- a/spec/files/small_list.xlsx
+++ b/spec/files/small_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="0" windowWidth="25600" windowHeight="27520" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -4502,9 +4502,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+      <selection pane="bottomLeft" activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5141,17 +5141,17 @@
       </c>
       <c r="I22" s="20"/>
       <c r="J22" s="3">
+        <v>-4</v>
+      </c>
+      <c r="K22" s="3">
         <v>4</v>
-      </c>
-      <c r="K22" s="3">
-        <v>-4</v>
       </c>
       <c r="L22" s="3">
         <v>0</v>
       </c>
       <c r="M22" s="3">
         <f>(K22-J22)/6</f>
-        <v>-1.3333333333333333</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
add openstudio server version. make real booleans.
</commit_message>
<xml_diff>
--- a/spec/files/small_list.xlsx
+++ b/spec/files/small_list.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="12816" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="12820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1844" uniqueCount="481">
   <si>
     <t>type</t>
   </si>
@@ -1467,6 +1467,12 @@
   </si>
   <si>
     <t>(double)</t>
+  </si>
+  <si>
+    <t>2 Cores</t>
+  </si>
+  <si>
+    <t>$0.410/hour</t>
   </si>
 </sst>
 </file>
@@ -1579,8 +1585,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1255">
+  <cellStyleXfs count="1259">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2900,7 +2910,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1255">
+  <cellStyles count="1259">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3528,6 +3538,8 @@
     <cellStyle name="Followed Hyperlink" xfId="1250" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1252" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1258" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4155,6 +4167,8 @@
     <cellStyle name="Hyperlink" xfId="1249" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1251" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1257" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4168,7 +4182,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Instructions"/>
@@ -4184,52 +4198,7 @@
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
-      <sheetData sheetId="5">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>m2.xlarge</v>
-          </cell>
-          <cell r="B2" t="str">
-            <v>2 Cores</v>
-          </cell>
-          <cell r="C2" t="str">
-            <v>$0.410/hour</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>m2.2xlarge</v>
-          </cell>
-          <cell r="B3" t="str">
-            <v>4 Cores</v>
-          </cell>
-          <cell r="C3" t="str">
-            <v>$0.820/hour</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>c3.2xlarge</v>
-          </cell>
-          <cell r="B4" t="str">
-            <v>8 Cores</v>
-          </cell>
-          <cell r="C4" t="str">
-            <v>$1.20/hour</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>cc2.8xlarge</v>
-          </cell>
-          <cell r="B5" t="str">
-            <v>16 Cores</v>
-          </cell>
-          <cell r="C5" t="str">
-            <v>$2.40/hour</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="5"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4528,17 +4497,17 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="50.77734375" customWidth="1"/>
+    <col min="1" max="1" width="50.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -4558,21 +4527,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.77734375" style="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="21"/>
       <c r="B1" s="22"/>
       <c r="C1" s="21"/>
@@ -4581,7 +4550,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="13" customFormat="1">
       <c r="A2" s="12" t="s">
         <v>452</v>
       </c>
@@ -4590,7 +4559,7 @@
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>453</v>
       </c>
@@ -4601,45 +4570,41 @@
         <v>455</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>456</v>
       </c>
       <c r="B4" s="25" t="s">
         <v>457</v>
       </c>
-      <c r="C4" s="3" t="str">
-        <f>INDEX([1]Lookups!$A$2:$C$5,MATCH($B4,[1]Lookups!$A$2:$A$5,0),2)</f>
-        <v>2 Cores</v>
-      </c>
-      <c r="D4" s="3" t="str">
-        <f>INDEX([1]Lookups!$A$2:$C$5,MATCH($B4,[1]Lookups!$A$2:$A$5,0),3)</f>
-        <v>$0.410/hour</v>
+      <c r="C4" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>480</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="28">
       <c r="A5" s="1" t="s">
         <v>459</v>
       </c>
       <c r="B5" s="25" t="s">
         <v>457</v>
       </c>
-      <c r="C5" s="3" t="str">
-        <f>INDEX([1]Lookups!$A$2:$C$5,MATCH($B5,[1]Lookups!$A$2:$A$5,0),2)</f>
-        <v>2 Cores</v>
-      </c>
-      <c r="D5" s="3" t="str">
-        <f>INDEX([1]Lookups!$A$2:$C$5,MATCH($B5,[1]Lookups!$A$2:$A$5,0),3)</f>
-        <v>$0.410/hour</v>
+      <c r="C5" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>480</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" s="13" customFormat="1">
       <c r="A7" s="12" t="s">
         <v>32</v>
       </c>
@@ -4648,7 +4613,7 @@
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -4659,7 +4624,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -4667,7 +4632,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -4675,7 +4640,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" s="2" customFormat="1" ht="42">
       <c r="A12" s="12" t="s">
         <v>31</v>
       </c>
@@ -4686,7 +4651,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
         <v>464</v>
       </c>
@@ -4694,7 +4659,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" s="2" customFormat="1" ht="42">
       <c r="A15" s="12" t="s">
         <v>465</v>
       </c>
@@ -4705,7 +4670,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -4713,7 +4678,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
@@ -4721,7 +4686,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>467</v>
       </c>
@@ -4730,7 +4695,7 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="20" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" s="2" customFormat="1" ht="28">
       <c r="A20" s="12" t="s">
         <v>38</v>
       </c>
@@ -4743,7 +4708,7 @@
       <c r="D20" s="12"/>
       <c r="E20" s="14"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
@@ -4751,7 +4716,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" s="2" customFormat="1" ht="28">
       <c r="A23" s="12" t="s">
         <v>34</v>
       </c>
@@ -4768,7 +4733,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="28">
       <c r="A24" s="1" t="s">
         <v>37</v>
       </c>
@@ -4785,7 +4750,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" s="2" customFormat="1" ht="42">
       <c r="A26" s="12" t="s">
         <v>40</v>
       </c>
@@ -4834,25 +4799,25 @@
       <selection pane="bottomLeft" activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="61.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="45.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="61.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="42.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" style="5"/>
-    <col min="10" max="15" width="11.44140625" style="1"/>
-    <col min="16" max="16" width="46.109375" style="1" customWidth="1"/>
-    <col min="17" max="19" width="11.44140625" style="1"/>
+    <col min="9" max="9" width="11.5" style="5"/>
+    <col min="10" max="15" width="11.5" style="1"/>
+    <col min="16" max="16" width="46.1640625" style="1" customWidth="1"/>
+    <col min="17" max="19" width="11.5" style="1"/>
     <col min="20" max="20" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="11.44140625" style="1"/>
+    <col min="21" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" ht="18">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="8" t="s">
@@ -4880,7 +4845,7 @@
       <c r="U1" s="27"/>
       <c r="V1" s="27"/>
     </row>
-    <row r="2" spans="1:22" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" s="9" customFormat="1" ht="15">
       <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
@@ -4893,7 +4858,7 @@
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:22" s="16" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" s="16" customFormat="1" ht="45">
       <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
@@ -4958,7 +4923,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22">
       <c r="A4" t="b">
         <v>1</v>
       </c>
@@ -4982,7 +4947,7 @@
       <c r="O4" s="4"/>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22">
       <c r="A5"/>
       <c r="B5" t="s">
         <v>24</v>
@@ -5013,7 +4978,7 @@
       <c r="O5" s="4"/>
       <c r="P5" s="2"/>
     </row>
-    <row r="6" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" ht="28">
       <c r="A6"/>
       <c r="B6" t="s">
         <v>25</v>
@@ -5055,7 +5020,7 @@
       </c>
       <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22">
       <c r="A7"/>
       <c r="B7" t="s">
         <v>24</v>
@@ -5083,7 +5048,7 @@
       <c r="O7" s="4"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22">
       <c r="A8"/>
       <c r="B8" t="s">
         <v>24</v>
@@ -5111,7 +5076,7 @@
       <c r="O8" s="4"/>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22">
       <c r="A9"/>
       <c r="B9" t="s">
         <v>24</v>
@@ -5139,7 +5104,7 @@
       <c r="O9" s="4"/>
       <c r="P9" s="2"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22">
       <c r="A10"/>
       <c r="B10" t="s">
         <v>24</v>
@@ -5169,7 +5134,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22">
       <c r="A11"/>
       <c r="B11" t="s">
         <v>24</v>
@@ -5197,7 +5162,7 @@
       <c r="O11" s="4"/>
       <c r="P11" s="2"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22">
       <c r="A12"/>
       <c r="B12" t="s">
         <v>24</v>
@@ -5225,7 +5190,7 @@
       <c r="O12" s="4"/>
       <c r="P12" s="2"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22">
       <c r="A13"/>
       <c r="B13" t="s">
         <v>24</v>
@@ -5253,7 +5218,7 @@
       <c r="O13" s="4"/>
       <c r="P13" s="2"/>
     </row>
-    <row r="14" spans="1:22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" customFormat="1">
       <c r="A14" t="b">
         <v>1</v>
       </c>
@@ -5267,7 +5232,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" customFormat="1">
       <c r="B15" t="s">
         <v>24</v>
       </c>
@@ -5290,7 +5255,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" customFormat="1">
       <c r="B16" t="s">
         <v>25</v>
       </c>
@@ -5327,7 +5292,7 @@
       </c>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" customFormat="1">
       <c r="B17" t="s">
         <v>24</v>
       </c>
@@ -5347,7 +5312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" customFormat="1">
       <c r="B18" t="s">
         <v>24</v>
       </c>
@@ -5367,7 +5332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" customFormat="1">
       <c r="B19" t="s">
         <v>24</v>
       </c>
@@ -5387,7 +5352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" customFormat="1" ht="15">
       <c r="A20" s="20" t="b">
         <v>1</v>
       </c>
@@ -5411,7 +5376,7 @@
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
     </row>
-    <row r="21" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" customFormat="1" ht="15">
       <c r="A21" s="20"/>
       <c r="B21" s="20" t="s">
         <v>25</v>
@@ -5450,7 +5415,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" customFormat="1" ht="15">
       <c r="A22" s="20"/>
       <c r="B22" s="20" t="s">
         <v>25</v>
@@ -5489,7 +5454,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" customFormat="1" ht="15">
       <c r="A23" s="20"/>
       <c r="B23" s="20" t="s">
         <v>24</v>
@@ -5512,7 +5477,7 @@
       </c>
       <c r="I23" s="20"/>
     </row>
-    <row r="24" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" customFormat="1" ht="15">
       <c r="A24" s="20" t="b">
         <v>1</v>
       </c>
@@ -5531,7 +5496,7 @@
       <c r="H24" s="20"/>
       <c r="I24" s="20"/>
     </row>
-    <row r="25" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" customFormat="1" ht="15">
       <c r="A25" s="20"/>
       <c r="B25" s="20" t="s">
         <v>25</v>
@@ -5570,7 +5535,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" customFormat="1" ht="15">
       <c r="A26" s="20"/>
       <c r="B26" s="20" t="s">
         <v>24</v>
@@ -5593,7 +5558,7 @@
       </c>
       <c r="I26" s="20"/>
     </row>
-    <row r="27" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" customFormat="1" ht="15">
       <c r="A27" s="20"/>
       <c r="B27" s="20" t="s">
         <v>24</v>
@@ -5616,7 +5581,7 @@
       </c>
       <c r="I27" s="20"/>
     </row>
-    <row r="28" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" customFormat="1" ht="15">
       <c r="A28" s="20"/>
       <c r="B28" s="20" t="s">
         <v>24</v>
@@ -5639,7 +5604,7 @@
       </c>
       <c r="I28" s="20"/>
     </row>
-    <row r="29" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" customFormat="1" ht="15">
       <c r="A29" s="20" t="b">
         <v>1</v>
       </c>
@@ -5658,7 +5623,7 @@
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
     </row>
-    <row r="30" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" customFormat="1" ht="15">
       <c r="A30" s="20"/>
       <c r="B30" s="20" t="s">
         <v>25</v>
@@ -5697,7 +5662,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" customFormat="1" ht="15">
       <c r="A31" s="20"/>
       <c r="B31" s="20" t="s">
         <v>24</v>
@@ -5720,7 +5685,7 @@
       </c>
       <c r="I31" s="20"/>
     </row>
-    <row r="32" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" customFormat="1" ht="15">
       <c r="A32" s="20"/>
       <c r="B32" s="20" t="s">
         <v>24</v>
@@ -5743,7 +5708,7 @@
       </c>
       <c r="I32" s="20"/>
     </row>
-    <row r="33" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" customFormat="1" ht="15">
       <c r="A33" s="20"/>
       <c r="B33" s="20" t="s">
         <v>24</v>
@@ -5766,7 +5731,7 @@
       </c>
       <c r="I33" s="20"/>
     </row>
-    <row r="34" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" customFormat="1" ht="15">
       <c r="A34" s="20" t="b">
         <v>1</v>
       </c>
@@ -5785,7 +5750,7 @@
       <c r="H34" s="20"/>
       <c r="I34" s="20"/>
     </row>
-    <row r="35" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" customFormat="1" ht="15">
       <c r="A35" s="20"/>
       <c r="B35" s="20" t="s">
         <v>24</v>
@@ -5810,7 +5775,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" customFormat="1" ht="15">
       <c r="A36" s="20"/>
       <c r="B36" s="20" t="s">
         <v>25</v>
@@ -5868,30 +5833,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="61.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="45.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="61.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="42.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" style="5"/>
-    <col min="10" max="15" width="11.44140625" style="1"/>
-    <col min="16" max="16" width="46.109375" style="1" customWidth="1"/>
-    <col min="17" max="19" width="11.44140625" style="1"/>
+    <col min="9" max="9" width="11.5" style="5"/>
+    <col min="10" max="15" width="11.5" style="1"/>
+    <col min="16" max="16" width="46.1640625" style="1" customWidth="1"/>
+    <col min="17" max="19" width="11.5" style="1"/>
     <col min="20" max="20" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="11.44140625" style="1"/>
+    <col min="21" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" ht="18">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="8" t="s">
@@ -5917,7 +5882,7 @@
       <c r="U1" s="27"/>
       <c r="V1" s="27"/>
     </row>
-    <row r="2" spans="1:22" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" s="9" customFormat="1" ht="15">
       <c r="A2" s="9" t="s">
         <v>472</v>
       </c>
@@ -5936,7 +5901,7 @@
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:22" s="16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" s="16" customFormat="1" ht="15">
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11" t="s">
@@ -5958,7 +5923,7 @@
       <c r="P3" s="11"/>
       <c r="Q3" s="11"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22">
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4"/>
@@ -5973,7 +5938,7 @@
       <c r="O4" s="4"/>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22">
       <c r="A5"/>
       <c r="B5"/>
       <c r="C5"/>
@@ -5990,7 +5955,7 @@
       <c r="O5" s="4"/>
       <c r="P5" s="2"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6"/>
@@ -6006,7 +5971,7 @@
       <c r="O6" s="4"/>
       <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7" s="15"/>
@@ -6022,7 +5987,7 @@
       <c r="O7" s="4"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8"/>
@@ -6038,7 +6003,7 @@
       <c r="O8" s="4"/>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9"/>
@@ -6054,7 +6019,7 @@
       <c r="O9" s="4"/>
       <c r="P9" s="2"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
@@ -6070,7 +6035,7 @@
       <c r="O10" s="4"/>
       <c r="P10"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
@@ -6086,7 +6051,7 @@
       <c r="O11" s="4"/>
       <c r="P11" s="2"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
@@ -6102,7 +6067,7 @@
       <c r="O12" s="4"/>
       <c r="P12" s="2"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
@@ -6118,9 +6083,9 @@
       <c r="O13" s="4"/>
       <c r="P13" s="2"/>
     </row>
-    <row r="14" spans="1:22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" customFormat="1"/>
+    <row r="15" spans="1:22" customFormat="1"/>
+    <row r="16" spans="1:22" customFormat="1">
       <c r="C16" s="19"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -6129,10 +6094,10 @@
       <c r="N16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:14" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:14" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="1:14" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" customFormat="1"/>
+    <row r="18" spans="1:14" customFormat="1"/>
+    <row r="19" spans="1:14" customFormat="1"/>
+    <row r="20" spans="1:14" customFormat="1" ht="15">
       <c r="A20" s="20"/>
       <c r="B20" s="20"/>
       <c r="C20" s="20"/>
@@ -6148,7 +6113,7 @@
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
     </row>
-    <row r="21" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" customFormat="1" ht="15">
       <c r="A21" s="20"/>
       <c r="B21" s="20"/>
       <c r="C21" s="20"/>
@@ -6164,7 +6129,7 @@
       <c r="M21" s="3"/>
       <c r="N21" s="1"/>
     </row>
-    <row r="22" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" customFormat="1" ht="15">
       <c r="A22" s="20"/>
       <c r="B22" s="20"/>
       <c r="C22" s="20"/>
@@ -6180,7 +6145,7 @@
       <c r="M22" s="3"/>
       <c r="N22" s="1"/>
     </row>
-    <row r="23" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" customFormat="1" ht="15">
       <c r="A23" s="20"/>
       <c r="B23" s="20"/>
       <c r="C23" s="20"/>
@@ -6191,7 +6156,7 @@
       <c r="H23" s="20"/>
       <c r="I23" s="20"/>
     </row>
-    <row r="24" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" customFormat="1" ht="15">
       <c r="A24" s="20"/>
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
@@ -6202,7 +6167,7 @@
       <c r="H24" s="20"/>
       <c r="I24" s="20"/>
     </row>
-    <row r="25" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" customFormat="1" ht="15">
       <c r="A25" s="20"/>
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
@@ -6216,7 +6181,7 @@
       <c r="M25" s="3"/>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" customFormat="1" ht="15">
       <c r="A26" s="20"/>
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
@@ -6227,7 +6192,7 @@
       <c r="H26" s="20"/>
       <c r="I26" s="20"/>
     </row>
-    <row r="27" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" customFormat="1" ht="15">
       <c r="A27" s="20"/>
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
@@ -6238,7 +6203,7 @@
       <c r="H27" s="20"/>
       <c r="I27" s="20"/>
     </row>
-    <row r="28" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" customFormat="1" ht="15">
       <c r="A28" s="20"/>
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>
@@ -6249,7 +6214,7 @@
       <c r="H28" s="20"/>
       <c r="I28" s="20"/>
     </row>
-    <row r="29" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" customFormat="1" ht="15">
       <c r="A29" s="20"/>
       <c r="B29" s="20"/>
       <c r="C29" s="20"/>
@@ -6260,7 +6225,7 @@
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
     </row>
-    <row r="30" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" customFormat="1" ht="15">
       <c r="A30" s="20"/>
       <c r="B30" s="20"/>
       <c r="C30" s="20"/>
@@ -6274,7 +6239,7 @@
       <c r="M30" s="3"/>
       <c r="N30" s="1"/>
     </row>
-    <row r="31" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" customFormat="1" ht="15">
       <c r="A31" s="20"/>
       <c r="B31" s="20"/>
       <c r="C31" s="20"/>
@@ -6285,7 +6250,7 @@
       <c r="H31" s="20"/>
       <c r="I31" s="20"/>
     </row>
-    <row r="32" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" customFormat="1" ht="15">
       <c r="A32" s="20"/>
       <c r="B32" s="20"/>
       <c r="C32" s="20"/>
@@ -6296,7 +6261,7 @@
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
     </row>
-    <row r="33" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" customFormat="1" ht="15">
       <c r="A33" s="20"/>
       <c r="B33" s="20"/>
       <c r="C33" s="20"/>
@@ -6307,7 +6272,7 @@
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
     </row>
-    <row r="34" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" customFormat="1" ht="15">
       <c r="A34" s="20"/>
       <c r="B34" s="20"/>
       <c r="C34" s="20"/>
@@ -6318,7 +6283,7 @@
       <c r="H34" s="20"/>
       <c r="I34" s="20"/>
     </row>
-    <row r="35" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" customFormat="1" ht="15">
       <c r="A35" s="20"/>
       <c r="B35" s="20"/>
       <c r="C35" s="20"/>
@@ -6329,7 +6294,7 @@
       <c r="H35" s="20"/>
       <c r="I35" s="20"/>
     </row>
-    <row r="36" spans="1:14" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" customFormat="1" ht="15">
       <c r="A36" s="20"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
@@ -6350,6 +6315,11 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6361,19 +6331,19 @@
       <selection activeCell="C253" sqref="C253"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="80.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15">
       <c r="A1" s="20" t="b">
         <v>0</v>
       </c>
@@ -6392,7 +6362,7 @@
       <c r="H1" s="20"/>
       <c r="I1" s="20"/>
     </row>
-    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15">
       <c r="A2" s="20"/>
       <c r="B2" s="20" t="s">
         <v>24</v>
@@ -6413,7 +6383,7 @@
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
     </row>
-    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15">
       <c r="A3" s="20"/>
       <c r="B3" s="20" t="s">
         <v>24</v>
@@ -6436,7 +6406,7 @@
       </c>
       <c r="I3" s="20"/>
     </row>
-    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15">
       <c r="A4" s="20"/>
       <c r="B4" s="20" t="s">
         <v>24</v>
@@ -6459,7 +6429,7 @@
       </c>
       <c r="I4" s="20"/>
     </row>
-    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15">
       <c r="A5" s="20"/>
       <c r="B5" s="20" t="s">
         <v>24</v>
@@ -6482,7 +6452,7 @@
       </c>
       <c r="I5" s="20"/>
     </row>
-    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15">
       <c r="A6" s="20"/>
       <c r="B6" s="20" t="s">
         <v>24</v>
@@ -6505,7 +6475,7 @@
       </c>
       <c r="I6" s="20"/>
     </row>
-    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15">
       <c r="A7" s="20"/>
       <c r="B7" s="20" t="s">
         <v>24</v>
@@ -6528,7 +6498,7 @@
       </c>
       <c r="I7" s="20"/>
     </row>
-    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="15">
       <c r="A8" s="20"/>
       <c r="B8" s="20" t="s">
         <v>24</v>
@@ -6551,7 +6521,7 @@
       </c>
       <c r="I8" s="20"/>
     </row>
-    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15">
       <c r="A9" s="20"/>
       <c r="B9" s="20" t="s">
         <v>24</v>
@@ -6574,7 +6544,7 @@
       </c>
       <c r="I9" s="20"/>
     </row>
-    <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="15">
       <c r="A10" s="20"/>
       <c r="B10" s="20" t="s">
         <v>24</v>
@@ -6597,7 +6567,7 @@
       </c>
       <c r="I10" s="20"/>
     </row>
-    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="15">
       <c r="A11" s="20" t="b">
         <v>0</v>
       </c>
@@ -6616,7 +6586,7 @@
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
     </row>
-    <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15">
       <c r="A12" s="20"/>
       <c r="B12" s="20" t="s">
         <v>24</v>
@@ -6637,7 +6607,7 @@
       <c r="H12" s="20"/>
       <c r="I12" s="20"/>
     </row>
-    <row r="13" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="15">
       <c r="A13" s="20"/>
       <c r="B13" s="20" t="s">
         <v>24</v>
@@ -6660,7 +6630,7 @@
       </c>
       <c r="I13" s="20"/>
     </row>
-    <row r="14" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="15">
       <c r="A14" s="20"/>
       <c r="B14" s="20" t="s">
         <v>24</v>
@@ -6683,7 +6653,7 @@
       </c>
       <c r="I14" s="20"/>
     </row>
-    <row r="15" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="15">
       <c r="A15" s="20"/>
       <c r="B15" s="20" t="s">
         <v>24</v>
@@ -6706,7 +6676,7 @@
       </c>
       <c r="I15" s="20"/>
     </row>
-    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="15">
       <c r="A16" s="20"/>
       <c r="B16" s="20" t="s">
         <v>24</v>
@@ -6729,7 +6699,7 @@
       </c>
       <c r="I16" s="20"/>
     </row>
-    <row r="17" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15">
       <c r="A17" s="20"/>
       <c r="B17" s="20" t="s">
         <v>24</v>
@@ -6752,7 +6722,7 @@
       </c>
       <c r="I17" s="20"/>
     </row>
-    <row r="18" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="15">
       <c r="A18" s="20"/>
       <c r="B18" s="20" t="s">
         <v>24</v>
@@ -6775,7 +6745,7 @@
       </c>
       <c r="I18" s="20"/>
     </row>
-    <row r="19" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="15">
       <c r="A19" s="20"/>
       <c r="B19" s="20" t="s">
         <v>24</v>
@@ -6798,7 +6768,7 @@
       </c>
       <c r="I19" s="20"/>
     </row>
-    <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15">
       <c r="A20" s="20"/>
       <c r="B20" s="20" t="s">
         <v>24</v>
@@ -6821,7 +6791,7 @@
       </c>
       <c r="I20" s="20"/>
     </row>
-    <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="15">
       <c r="A21" s="20" t="b">
         <v>0</v>
       </c>
@@ -6840,7 +6810,7 @@
       <c r="H21" s="20"/>
       <c r="I21" s="20"/>
     </row>
-    <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="15">
       <c r="A22" s="20"/>
       <c r="B22" s="20" t="s">
         <v>24</v>
@@ -6863,7 +6833,7 @@
       </c>
       <c r="I22" s="20"/>
     </row>
-    <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="15">
       <c r="A23" s="20"/>
       <c r="B23" s="20" t="s">
         <v>24</v>
@@ -6886,7 +6856,7 @@
       </c>
       <c r="I23" s="20"/>
     </row>
-    <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="15">
       <c r="A24" s="20"/>
       <c r="B24" s="20" t="s">
         <v>24</v>
@@ -6909,7 +6879,7 @@
       </c>
       <c r="I24" s="20"/>
     </row>
-    <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15">
       <c r="A25" s="20"/>
       <c r="B25" s="20" t="s">
         <v>24</v>
@@ -6932,7 +6902,7 @@
       </c>
       <c r="I25" s="20"/>
     </row>
-    <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="15">
       <c r="A26" s="20"/>
       <c r="B26" s="20" t="s">
         <v>24</v>
@@ -6955,7 +6925,7 @@
       </c>
       <c r="I26" s="20"/>
     </row>
-    <row r="27" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="15">
       <c r="A27" s="20"/>
       <c r="B27" s="20" t="s">
         <v>24</v>
@@ -6978,7 +6948,7 @@
       </c>
       <c r="I27" s="20"/>
     </row>
-    <row r="28" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="15">
       <c r="A28" s="20"/>
       <c r="B28" s="20" t="s">
         <v>24</v>
@@ -7001,7 +6971,7 @@
       </c>
       <c r="I28" s="20"/>
     </row>
-    <row r="29" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="15">
       <c r="A29" s="20"/>
       <c r="B29" s="20" t="s">
         <v>24</v>
@@ -7024,7 +6994,7 @@
       </c>
       <c r="I29" s="20"/>
     </row>
-    <row r="30" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="15">
       <c r="A30" s="20"/>
       <c r="B30" s="20" t="s">
         <v>24</v>
@@ -7047,7 +7017,7 @@
       </c>
       <c r="I30" s="20"/>
     </row>
-    <row r="31" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="15">
       <c r="A31" s="20" t="b">
         <v>0</v>
       </c>
@@ -7066,7 +7036,7 @@
       <c r="H31" s="20"/>
       <c r="I31" s="20"/>
     </row>
-    <row r="32" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="15">
       <c r="A32" s="20"/>
       <c r="B32" s="20" t="s">
         <v>24</v>
@@ -7087,7 +7057,7 @@
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
     </row>
-    <row r="33" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="15">
       <c r="A33" s="20"/>
       <c r="B33" s="20" t="s">
         <v>24</v>
@@ -7110,7 +7080,7 @@
       </c>
       <c r="I33" s="20"/>
     </row>
-    <row r="34" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="15">
       <c r="A34" s="20"/>
       <c r="B34" s="20" t="s">
         <v>24</v>
@@ -7133,7 +7103,7 @@
       </c>
       <c r="I34" s="20"/>
     </row>
-    <row r="35" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="15">
       <c r="A35" s="20"/>
       <c r="B35" s="20" t="s">
         <v>24</v>
@@ -7156,7 +7126,7 @@
       </c>
       <c r="I35" s="20"/>
     </row>
-    <row r="36" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="15">
       <c r="A36" s="20"/>
       <c r="B36" s="20" t="s">
         <v>24</v>
@@ -7179,7 +7149,7 @@
       </c>
       <c r="I36" s="20"/>
     </row>
-    <row r="37" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="15">
       <c r="A37" s="20"/>
       <c r="B37" s="20" t="s">
         <v>24</v>
@@ -7202,7 +7172,7 @@
       </c>
       <c r="I37" s="20"/>
     </row>
-    <row r="38" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="15">
       <c r="A38" s="20"/>
       <c r="B38" s="20" t="s">
         <v>24</v>
@@ -7225,7 +7195,7 @@
       </c>
       <c r="I38" s="20"/>
     </row>
-    <row r="39" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="15">
       <c r="A39" s="20"/>
       <c r="B39" s="20" t="s">
         <v>24</v>
@@ -7248,7 +7218,7 @@
       </c>
       <c r="I39" s="20"/>
     </row>
-    <row r="40" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="15">
       <c r="A40" s="20"/>
       <c r="B40" s="20" t="s">
         <v>24</v>
@@ -7271,7 +7241,7 @@
       </c>
       <c r="I40" s="20"/>
     </row>
-    <row r="41" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="15">
       <c r="A41" s="20" t="b">
         <v>0</v>
       </c>
@@ -7290,7 +7260,7 @@
       <c r="H41" s="20"/>
       <c r="I41" s="20"/>
     </row>
-    <row r="42" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="15">
       <c r="A42" s="20"/>
       <c r="B42" s="20" t="s">
         <v>24</v>
@@ -7311,7 +7281,7 @@
       <c r="H42" s="20"/>
       <c r="I42" s="20"/>
     </row>
-    <row r="43" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="15">
       <c r="A43" s="20"/>
       <c r="B43" s="20" t="s">
         <v>24</v>
@@ -7334,7 +7304,7 @@
       </c>
       <c r="I43" s="20"/>
     </row>
-    <row r="44" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="15">
       <c r="A44" s="20"/>
       <c r="B44" s="20" t="s">
         <v>24</v>
@@ -7357,7 +7327,7 @@
       </c>
       <c r="I44" s="20"/>
     </row>
-    <row r="45" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="15">
       <c r="A45" s="20"/>
       <c r="B45" s="20" t="s">
         <v>24</v>
@@ -7380,7 +7350,7 @@
       </c>
       <c r="I45" s="20"/>
     </row>
-    <row r="46" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="15">
       <c r="A46" s="20"/>
       <c r="B46" s="20" t="s">
         <v>24</v>
@@ -7403,7 +7373,7 @@
       </c>
       <c r="I46" s="20"/>
     </row>
-    <row r="47" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="15">
       <c r="A47" s="20"/>
       <c r="B47" s="20" t="s">
         <v>24</v>
@@ -7426,7 +7396,7 @@
       </c>
       <c r="I47" s="20"/>
     </row>
-    <row r="48" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="15">
       <c r="A48" s="20"/>
       <c r="B48" s="20" t="s">
         <v>24</v>
@@ -7449,7 +7419,7 @@
       </c>
       <c r="I48" s="20"/>
     </row>
-    <row r="49" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="15">
       <c r="A49" s="20"/>
       <c r="B49" s="20" t="s">
         <v>24</v>
@@ -7472,7 +7442,7 @@
       </c>
       <c r="I49" s="20"/>
     </row>
-    <row r="50" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="15">
       <c r="A50" s="20"/>
       <c r="B50" s="20" t="s">
         <v>24</v>
@@ -7495,7 +7465,7 @@
       </c>
       <c r="I50" s="20"/>
     </row>
-    <row r="51" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="15">
       <c r="A51" s="20" t="b">
         <v>0</v>
       </c>
@@ -7514,7 +7484,7 @@
       <c r="H51" s="20"/>
       <c r="I51" s="20"/>
     </row>
-    <row r="52" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="15">
       <c r="A52" s="20"/>
       <c r="B52" s="20" t="s">
         <v>24</v>
@@ -7535,7 +7505,7 @@
       <c r="H52" s="20"/>
       <c r="I52" s="20"/>
     </row>
-    <row r="53" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="15">
       <c r="A53" s="20"/>
       <c r="B53" s="20" t="s">
         <v>24</v>
@@ -7558,7 +7528,7 @@
       </c>
       <c r="I53" s="20"/>
     </row>
-    <row r="54" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="15">
       <c r="A54" s="20"/>
       <c r="B54" s="20" t="s">
         <v>24</v>
@@ -7581,7 +7551,7 @@
       </c>
       <c r="I54" s="20"/>
     </row>
-    <row r="55" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="15">
       <c r="A55" s="20"/>
       <c r="B55" s="20" t="s">
         <v>24</v>
@@ -7604,7 +7574,7 @@
       </c>
       <c r="I55" s="20"/>
     </row>
-    <row r="56" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="15">
       <c r="A56" s="20"/>
       <c r="B56" s="20" t="s">
         <v>24</v>
@@ -7627,7 +7597,7 @@
       </c>
       <c r="I56" s="20"/>
     </row>
-    <row r="57" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="15">
       <c r="A57" s="20"/>
       <c r="B57" s="20" t="s">
         <v>24</v>
@@ -7650,7 +7620,7 @@
       </c>
       <c r="I57" s="20"/>
     </row>
-    <row r="58" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="15">
       <c r="A58" s="20"/>
       <c r="B58" s="20" t="s">
         <v>24</v>
@@ -7673,7 +7643,7 @@
       </c>
       <c r="I58" s="20"/>
     </row>
-    <row r="59" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="15">
       <c r="A59" s="20"/>
       <c r="B59" s="20" t="s">
         <v>24</v>
@@ -7696,7 +7666,7 @@
       </c>
       <c r="I59" s="20"/>
     </row>
-    <row r="60" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="15">
       <c r="A60" s="20"/>
       <c r="B60" s="20" t="s">
         <v>24</v>
@@ -7719,7 +7689,7 @@
       </c>
       <c r="I60" s="20"/>
     </row>
-    <row r="61" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="15">
       <c r="A61" s="20" t="b">
         <v>0</v>
       </c>
@@ -7738,7 +7708,7 @@
       <c r="H61" s="20"/>
       <c r="I61" s="20"/>
     </row>
-    <row r="62" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" ht="15">
       <c r="A62" s="20"/>
       <c r="B62" s="20" t="s">
         <v>24</v>
@@ -7759,7 +7729,7 @@
       <c r="H62" s="20"/>
       <c r="I62" s="20"/>
     </row>
-    <row r="63" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="15">
       <c r="A63" s="20"/>
       <c r="B63" s="20" t="s">
         <v>24</v>
@@ -7784,7 +7754,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="15">
       <c r="A64" s="20"/>
       <c r="B64" s="20" t="s">
         <v>24</v>
@@ -7807,7 +7777,7 @@
       </c>
       <c r="I64" s="20"/>
     </row>
-    <row r="65" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" ht="15">
       <c r="A65" s="20"/>
       <c r="B65" s="20" t="s">
         <v>24</v>
@@ -7830,7 +7800,7 @@
       </c>
       <c r="I65" s="20"/>
     </row>
-    <row r="66" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" ht="15">
       <c r="A66" s="20"/>
       <c r="B66" s="20" t="s">
         <v>24</v>
@@ -7853,7 +7823,7 @@
       </c>
       <c r="I66" s="20"/>
     </row>
-    <row r="67" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" ht="15">
       <c r="A67" s="20"/>
       <c r="B67" s="20" t="s">
         <v>24</v>
@@ -7876,7 +7846,7 @@
       </c>
       <c r="I67" s="20"/>
     </row>
-    <row r="68" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" ht="15">
       <c r="A68" s="20"/>
       <c r="B68" s="20" t="s">
         <v>24</v>
@@ -7899,7 +7869,7 @@
       </c>
       <c r="I68" s="20"/>
     </row>
-    <row r="69" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" ht="15">
       <c r="A69" s="20"/>
       <c r="B69" s="20" t="s">
         <v>24</v>
@@ -7922,7 +7892,7 @@
       </c>
       <c r="I69" s="20"/>
     </row>
-    <row r="70" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" ht="15">
       <c r="A70" s="20"/>
       <c r="B70" s="20" t="s">
         <v>24</v>
@@ -7945,7 +7915,7 @@
       </c>
       <c r="I70" s="20"/>
     </row>
-    <row r="71" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" ht="15">
       <c r="A71" s="20"/>
       <c r="B71" s="20" t="s">
         <v>24</v>
@@ -7968,7 +7938,7 @@
       </c>
       <c r="I71" s="20"/>
     </row>
-    <row r="72" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" ht="15">
       <c r="A72" s="20" t="b">
         <v>0</v>
       </c>
@@ -7987,7 +7957,7 @@
       <c r="H72" s="20"/>
       <c r="I72" s="20"/>
     </row>
-    <row r="73" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" ht="15">
       <c r="A73" s="20"/>
       <c r="B73" s="20" t="s">
         <v>24</v>
@@ -8008,7 +7978,7 @@
       <c r="H73" s="20"/>
       <c r="I73" s="20"/>
     </row>
-    <row r="74" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" ht="15">
       <c r="A74" s="20"/>
       <c r="B74" s="20" t="s">
         <v>24</v>
@@ -8031,7 +8001,7 @@
       </c>
       <c r="I74" s="20"/>
     </row>
-    <row r="75" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" ht="15">
       <c r="A75" s="20"/>
       <c r="B75" s="20" t="s">
         <v>24</v>
@@ -8056,7 +8026,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" ht="15">
       <c r="A76" s="20"/>
       <c r="B76" s="20" t="s">
         <v>24</v>
@@ -8079,7 +8049,7 @@
       </c>
       <c r="I76" s="20"/>
     </row>
-    <row r="77" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" ht="15">
       <c r="A77" s="20"/>
       <c r="B77" s="20" t="s">
         <v>24</v>
@@ -8102,7 +8072,7 @@
       </c>
       <c r="I77" s="20"/>
     </row>
-    <row r="78" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" ht="15">
       <c r="A78" s="20"/>
       <c r="B78" s="20" t="s">
         <v>24</v>
@@ -8125,7 +8095,7 @@
       </c>
       <c r="I78" s="20"/>
     </row>
-    <row r="79" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" ht="15">
       <c r="A79" s="20"/>
       <c r="B79" s="20" t="s">
         <v>24</v>
@@ -8148,7 +8118,7 @@
       </c>
       <c r="I79" s="20"/>
     </row>
-    <row r="80" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" ht="15">
       <c r="A80" s="20"/>
       <c r="B80" s="20" t="s">
         <v>24</v>
@@ -8171,7 +8141,7 @@
       </c>
       <c r="I80" s="20"/>
     </row>
-    <row r="81" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" ht="15">
       <c r="A81" s="20"/>
       <c r="B81" s="20" t="s">
         <v>24</v>
@@ -8194,7 +8164,7 @@
       </c>
       <c r="I81" s="20"/>
     </row>
-    <row r="82" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" ht="15">
       <c r="A82" s="20"/>
       <c r="B82" s="20" t="s">
         <v>24</v>
@@ -8217,7 +8187,7 @@
       </c>
       <c r="I82" s="20"/>
     </row>
-    <row r="83" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" ht="15">
       <c r="A83" s="20"/>
       <c r="B83" s="20" t="s">
         <v>24</v>
@@ -8240,7 +8210,7 @@
       </c>
       <c r="I83" s="20"/>
     </row>
-    <row r="84" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" ht="15">
       <c r="A84" s="20"/>
       <c r="B84" s="20" t="s">
         <v>24</v>
@@ -8263,7 +8233,7 @@
       </c>
       <c r="I84" s="20"/>
     </row>
-    <row r="85" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" ht="15">
       <c r="A85" s="20"/>
       <c r="B85" s="20" t="s">
         <v>24</v>
@@ -8286,7 +8256,7 @@
       </c>
       <c r="I85" s="20"/>
     </row>
-    <row r="86" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" ht="15">
       <c r="A86" s="20" t="b">
         <v>0</v>
       </c>
@@ -8305,7 +8275,7 @@
       <c r="H86" s="20"/>
       <c r="I86" s="20"/>
     </row>
-    <row r="87" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" ht="15">
       <c r="A87" s="20"/>
       <c r="B87" s="20" t="s">
         <v>24</v>
@@ -8328,7 +8298,7 @@
       </c>
       <c r="I87" s="20"/>
     </row>
-    <row r="88" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" ht="15">
       <c r="A88" s="20"/>
       <c r="B88" s="20" t="s">
         <v>24</v>
@@ -8351,7 +8321,7 @@
       </c>
       <c r="I88" s="20"/>
     </row>
-    <row r="89" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" ht="15">
       <c r="A89" s="20"/>
       <c r="B89" s="20" t="s">
         <v>24</v>
@@ -8374,7 +8344,7 @@
       </c>
       <c r="I89" s="20"/>
     </row>
-    <row r="90" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" ht="15">
       <c r="A90" s="20"/>
       <c r="B90" s="20" t="s">
         <v>24</v>
@@ -8397,7 +8367,7 @@
       </c>
       <c r="I90" s="20"/>
     </row>
-    <row r="91" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" ht="15">
       <c r="A91" s="20"/>
       <c r="B91" s="20" t="s">
         <v>24</v>
@@ -8420,7 +8390,7 @@
       </c>
       <c r="I91" s="20"/>
     </row>
-    <row r="92" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" ht="15">
       <c r="A92" s="20"/>
       <c r="B92" s="20" t="s">
         <v>24</v>
@@ -8443,7 +8413,7 @@
       </c>
       <c r="I92" s="20"/>
     </row>
-    <row r="93" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" ht="15">
       <c r="A93" s="20"/>
       <c r="B93" s="20" t="s">
         <v>24</v>
@@ -8466,7 +8436,7 @@
       </c>
       <c r="I93" s="20"/>
     </row>
-    <row r="94" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" ht="15">
       <c r="A94" s="20"/>
       <c r="B94" s="20" t="s">
         <v>24</v>
@@ -8489,7 +8459,7 @@
       </c>
       <c r="I94" s="20"/>
     </row>
-    <row r="95" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" ht="15">
       <c r="A95" s="20"/>
       <c r="B95" s="20" t="s">
         <v>24</v>
@@ -8512,7 +8482,7 @@
       </c>
       <c r="I95" s="20"/>
     </row>
-    <row r="96" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" ht="15">
       <c r="A96" s="20"/>
       <c r="B96" s="20" t="s">
         <v>24</v>
@@ -8535,7 +8505,7 @@
       </c>
       <c r="I96" s="20"/>
     </row>
-    <row r="97" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" ht="15">
       <c r="A97" s="20" t="b">
         <v>0</v>
       </c>
@@ -8554,7 +8524,7 @@
       <c r="H97" s="20"/>
       <c r="I97" s="20"/>
     </row>
-    <row r="98" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" ht="15">
       <c r="A98" s="20"/>
       <c r="B98" s="20" t="s">
         <v>24</v>
@@ -8579,7 +8549,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" ht="15">
       <c r="A99" s="20" t="b">
         <v>0</v>
       </c>
@@ -8598,7 +8568,7 @@
       <c r="H99" s="20"/>
       <c r="I99" s="20"/>
     </row>
-    <row r="100" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" ht="15">
       <c r="A100" s="20"/>
       <c r="B100" s="20" t="s">
         <v>24</v>
@@ -8619,7 +8589,7 @@
       <c r="H100" s="20"/>
       <c r="I100" s="20"/>
     </row>
-    <row r="101" spans="1:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" ht="19" customHeight="1">
       <c r="A101" s="20"/>
       <c r="B101" s="20" t="s">
         <v>24</v>
@@ -8644,7 +8614,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" ht="15">
       <c r="A102" s="20" t="b">
         <v>0</v>
       </c>
@@ -8663,7 +8633,7 @@
       <c r="H102" s="20"/>
       <c r="I102" s="20"/>
     </row>
-    <row r="103" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" ht="15">
       <c r="A103" s="20"/>
       <c r="B103" s="20" t="s">
         <v>24</v>
@@ -8686,7 +8656,7 @@
       </c>
       <c r="I103" s="20"/>
     </row>
-    <row r="104" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" ht="15">
       <c r="A104" s="20"/>
       <c r="B104" s="20" t="s">
         <v>24</v>
@@ -8711,7 +8681,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" ht="15">
       <c r="A105" s="20"/>
       <c r="B105" s="20" t="s">
         <v>24</v>
@@ -8734,7 +8704,7 @@
       </c>
       <c r="I105" s="20"/>
     </row>
-    <row r="106" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" ht="15">
       <c r="A106" s="20"/>
       <c r="B106" s="20" t="s">
         <v>24</v>
@@ -8755,7 +8725,7 @@
       <c r="H106" s="20"/>
       <c r="I106" s="20"/>
     </row>
-    <row r="107" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" ht="15">
       <c r="A107" s="20" t="b">
         <v>0</v>
       </c>
@@ -8774,7 +8744,7 @@
       <c r="H107" s="20"/>
       <c r="I107" s="20"/>
     </row>
-    <row r="108" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" ht="15">
       <c r="A108" s="20"/>
       <c r="B108" s="20" t="s">
         <v>24</v>
@@ -8799,7 +8769,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" ht="15">
       <c r="A109" s="20"/>
       <c r="B109" s="20" t="s">
         <v>24</v>
@@ -8822,7 +8792,7 @@
       </c>
       <c r="I109" s="20"/>
     </row>
-    <row r="110" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" ht="15">
       <c r="A110" s="20"/>
       <c r="B110" s="20" t="s">
         <v>24</v>
@@ -8845,7 +8815,7 @@
       </c>
       <c r="I110" s="20"/>
     </row>
-    <row r="111" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" ht="15">
       <c r="A111" s="20"/>
       <c r="B111" s="20" t="s">
         <v>24</v>
@@ -8868,7 +8838,7 @@
       </c>
       <c r="I111" s="20"/>
     </row>
-    <row r="112" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" ht="15">
       <c r="A112" s="20"/>
       <c r="B112" s="20" t="s">
         <v>24</v>
@@ -8891,7 +8861,7 @@
       </c>
       <c r="I112" s="20"/>
     </row>
-    <row r="113" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" ht="15">
       <c r="A113" s="20"/>
       <c r="B113" s="20" t="s">
         <v>24</v>
@@ -8914,7 +8884,7 @@
       </c>
       <c r="I113" s="20"/>
     </row>
-    <row r="114" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" ht="15">
       <c r="A114" s="20"/>
       <c r="B114" s="20" t="s">
         <v>24</v>
@@ -8937,7 +8907,7 @@
       </c>
       <c r="I114" s="20"/>
     </row>
-    <row r="115" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" ht="15">
       <c r="A115" s="20" t="b">
         <v>0</v>
       </c>
@@ -8956,7 +8926,7 @@
       <c r="H115" s="20"/>
       <c r="I115" s="20"/>
     </row>
-    <row r="116" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" ht="15">
       <c r="A116" s="20"/>
       <c r="B116" s="20" t="s">
         <v>24</v>
@@ -8979,7 +8949,7 @@
       </c>
       <c r="I116" s="20"/>
     </row>
-    <row r="117" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" ht="15">
       <c r="A117" s="20"/>
       <c r="B117" s="20" t="s">
         <v>24</v>
@@ -9002,7 +8972,7 @@
       </c>
       <c r="I117" s="20"/>
     </row>
-    <row r="118" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" ht="15">
       <c r="A118" s="20"/>
       <c r="B118" s="20" t="s">
         <v>24</v>
@@ -9025,7 +8995,7 @@
       </c>
       <c r="I118" s="20"/>
     </row>
-    <row r="119" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" ht="15">
       <c r="A119" s="20" t="b">
         <v>0</v>
       </c>
@@ -9044,7 +9014,7 @@
       <c r="H119" s="20"/>
       <c r="I119" s="20"/>
     </row>
-    <row r="120" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" ht="15">
       <c r="A120" s="20"/>
       <c r="B120" s="20" t="s">
         <v>24</v>
@@ -9067,7 +9037,7 @@
       </c>
       <c r="I120" s="20"/>
     </row>
-    <row r="121" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" ht="15">
       <c r="A121" s="20"/>
       <c r="B121" s="20" t="s">
         <v>24</v>
@@ -9090,7 +9060,7 @@
       </c>
       <c r="I121" s="20"/>
     </row>
-    <row r="122" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" ht="15">
       <c r="A122" s="20"/>
       <c r="B122" s="20" t="s">
         <v>24</v>
@@ -9113,7 +9083,7 @@
       </c>
       <c r="I122" s="20"/>
     </row>
-    <row r="123" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" ht="15">
       <c r="A123" s="20"/>
       <c r="B123" s="20" t="s">
         <v>24</v>
@@ -9136,7 +9106,7 @@
       </c>
       <c r="I123" s="20"/>
     </row>
-    <row r="124" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" ht="15">
       <c r="A124" s="20"/>
       <c r="B124" s="20" t="s">
         <v>24</v>
@@ -9159,7 +9129,7 @@
       </c>
       <c r="I124" s="20"/>
     </row>
-    <row r="125" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" ht="15">
       <c r="A125" s="20"/>
       <c r="B125" s="20" t="s">
         <v>24</v>
@@ -9182,7 +9152,7 @@
       </c>
       <c r="I125" s="20"/>
     </row>
-    <row r="126" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" ht="15">
       <c r="A126" s="20" t="b">
         <v>0</v>
       </c>
@@ -9201,7 +9171,7 @@
       <c r="H126" s="20"/>
       <c r="I126" s="20"/>
     </row>
-    <row r="127" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" ht="15">
       <c r="A127" s="20"/>
       <c r="B127" s="20" t="s">
         <v>24</v>
@@ -9226,7 +9196,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" ht="15">
       <c r="A128" s="20"/>
       <c r="B128" s="20" t="s">
         <v>24</v>
@@ -9249,7 +9219,7 @@
       </c>
       <c r="I128" s="20"/>
     </row>
-    <row r="129" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" ht="15">
       <c r="A129" s="20"/>
       <c r="B129" s="20" t="s">
         <v>24</v>
@@ -9272,7 +9242,7 @@
       </c>
       <c r="I129" s="20"/>
     </row>
-    <row r="130" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" ht="15">
       <c r="A130" s="20"/>
       <c r="B130" s="20" t="s">
         <v>24</v>
@@ -9295,7 +9265,7 @@
       </c>
       <c r="I130" s="20"/>
     </row>
-    <row r="131" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:9" ht="15">
       <c r="A131" s="20"/>
       <c r="B131" s="20" t="s">
         <v>24</v>
@@ -9318,7 +9288,7 @@
       </c>
       <c r="I131" s="20"/>
     </row>
-    <row r="132" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9" ht="15">
       <c r="A132" s="20"/>
       <c r="B132" s="20" t="s">
         <v>24</v>
@@ -9341,7 +9311,7 @@
       </c>
       <c r="I132" s="20"/>
     </row>
-    <row r="133" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:9" ht="15">
       <c r="A133" s="20"/>
       <c r="B133" s="20" t="s">
         <v>24</v>
@@ -9364,7 +9334,7 @@
       </c>
       <c r="I133" s="20"/>
     </row>
-    <row r="134" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:9" ht="15">
       <c r="A134" s="20"/>
       <c r="B134" s="20" t="s">
         <v>24</v>
@@ -9387,7 +9357,7 @@
       </c>
       <c r="I134" s="20"/>
     </row>
-    <row r="135" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:9" ht="15">
       <c r="A135" s="20"/>
       <c r="B135" s="20" t="s">
         <v>24</v>
@@ -9410,7 +9380,7 @@
       </c>
       <c r="I135" s="20"/>
     </row>
-    <row r="136" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:9" ht="15">
       <c r="A136" s="20" t="b">
         <v>0</v>
       </c>
@@ -9429,7 +9399,7 @@
       <c r="H136" s="20"/>
       <c r="I136" s="20"/>
     </row>
-    <row r="137" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:9" ht="15">
       <c r="A137" s="20"/>
       <c r="B137" s="20" t="s">
         <v>24</v>
@@ -9454,7 +9424,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:9" ht="15">
       <c r="A138" s="20"/>
       <c r="B138" s="20" t="s">
         <v>24</v>
@@ -9475,7 +9445,7 @@
       <c r="H138" s="20"/>
       <c r="I138" s="20"/>
     </row>
-    <row r="139" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:9" ht="15">
       <c r="A139" s="20"/>
       <c r="B139" s="20" t="s">
         <v>24</v>
@@ -9498,7 +9468,7 @@
       </c>
       <c r="I139" s="20"/>
     </row>
-    <row r="140" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:9" ht="15">
       <c r="A140" s="20"/>
       <c r="B140" s="20" t="s">
         <v>24</v>
@@ -9521,7 +9491,7 @@
       </c>
       <c r="I140" s="20"/>
     </row>
-    <row r="141" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:9" ht="15">
       <c r="A141" s="20"/>
       <c r="B141" s="20" t="s">
         <v>24</v>
@@ -9544,7 +9514,7 @@
       </c>
       <c r="I141" s="20"/>
     </row>
-    <row r="142" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:9" ht="15">
       <c r="A142" s="20"/>
       <c r="B142" s="20" t="s">
         <v>24</v>
@@ -9567,7 +9537,7 @@
       </c>
       <c r="I142" s="20"/>
     </row>
-    <row r="143" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:9" ht="15">
       <c r="A143" s="20"/>
       <c r="B143" s="20" t="s">
         <v>24</v>
@@ -9590,7 +9560,7 @@
       </c>
       <c r="I143" s="20"/>
     </row>
-    <row r="144" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:9" ht="15">
       <c r="A144" s="20"/>
       <c r="B144" s="20" t="s">
         <v>24</v>
@@ -9613,7 +9583,7 @@
       </c>
       <c r="I144" s="20"/>
     </row>
-    <row r="145" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9" ht="15">
       <c r="A145" s="20"/>
       <c r="B145" s="20" t="s">
         <v>24</v>
@@ -9636,7 +9606,7 @@
       </c>
       <c r="I145" s="20"/>
     </row>
-    <row r="146" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" ht="15">
       <c r="A146" s="20"/>
       <c r="B146" s="20" t="s">
         <v>24</v>
@@ -9659,7 +9629,7 @@
       </c>
       <c r="I146" s="20"/>
     </row>
-    <row r="147" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" ht="15">
       <c r="A147" s="20"/>
       <c r="B147" s="20" t="s">
         <v>24</v>
@@ -9682,7 +9652,7 @@
       </c>
       <c r="I147" s="20"/>
     </row>
-    <row r="148" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:9" ht="15">
       <c r="A148" s="20"/>
       <c r="B148" s="20" t="s">
         <v>24</v>
@@ -9705,7 +9675,7 @@
       </c>
       <c r="I148" s="20"/>
     </row>
-    <row r="149" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9" ht="15">
       <c r="A149" s="20"/>
       <c r="B149" s="20" t="s">
         <v>24</v>
@@ -9728,7 +9698,7 @@
       </c>
       <c r="I149" s="20"/>
     </row>
-    <row r="150" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9" ht="15">
       <c r="A150" s="20"/>
       <c r="B150" s="20" t="s">
         <v>24</v>
@@ -9751,7 +9721,7 @@
       </c>
       <c r="I150" s="20"/>
     </row>
-    <row r="151" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9" ht="15">
       <c r="A151" s="20" t="b">
         <v>0</v>
       </c>
@@ -9770,7 +9740,7 @@
       <c r="H151" s="20"/>
       <c r="I151" s="20"/>
     </row>
-    <row r="152" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:9" ht="15">
       <c r="A152" s="20"/>
       <c r="B152" s="20" t="s">
         <v>24</v>
@@ -9793,7 +9763,7 @@
       </c>
       <c r="I152" s="20"/>
     </row>
-    <row r="153" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:9" ht="15">
       <c r="A153" s="20" t="b">
         <v>0</v>
       </c>
@@ -9812,7 +9782,7 @@
       <c r="H153" s="20"/>
       <c r="I153" s="20"/>
     </row>
-    <row r="154" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:9" ht="15">
       <c r="A154" s="20"/>
       <c r="B154" s="20" t="s">
         <v>24</v>
@@ -9835,7 +9805,7 @@
       </c>
       <c r="I154" s="20"/>
     </row>
-    <row r="155" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:9" ht="15">
       <c r="A155" s="20"/>
       <c r="B155" s="20" t="s">
         <v>24</v>
@@ -9858,7 +9828,7 @@
       </c>
       <c r="I155" s="20"/>
     </row>
-    <row r="156" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:9" ht="15">
       <c r="A156" s="20" t="b">
         <v>0</v>
       </c>
@@ -9877,7 +9847,7 @@
       <c r="H156" s="20"/>
       <c r="I156" s="20"/>
     </row>
-    <row r="157" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:9" ht="15">
       <c r="A157" s="20"/>
       <c r="B157" s="20" t="s">
         <v>24</v>
@@ -9902,7 +9872,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="158" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:9" ht="15">
       <c r="A158" s="20"/>
       <c r="B158" s="20" t="s">
         <v>24</v>
@@ -9925,7 +9895,7 @@
       </c>
       <c r="I158" s="20"/>
     </row>
-    <row r="159" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:9" ht="15">
       <c r="A159" s="20"/>
       <c r="B159" s="20" t="s">
         <v>24</v>
@@ -9948,7 +9918,7 @@
       </c>
       <c r="I159" s="20"/>
     </row>
-    <row r="160" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:9" ht="15">
       <c r="A160" s="20"/>
       <c r="B160" s="20" t="s">
         <v>24</v>
@@ -9971,7 +9941,7 @@
       </c>
       <c r="I160" s="20"/>
     </row>
-    <row r="161" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:9" ht="15">
       <c r="A161" s="20"/>
       <c r="B161" s="20" t="s">
         <v>24</v>
@@ -9994,7 +9964,7 @@
       </c>
       <c r="I161" s="20"/>
     </row>
-    <row r="162" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:9" ht="15">
       <c r="A162" s="20"/>
       <c r="B162" s="20" t="s">
         <v>24</v>
@@ -10017,7 +9987,7 @@
       </c>
       <c r="I162" s="20"/>
     </row>
-    <row r="163" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:9" ht="15">
       <c r="A163" s="20"/>
       <c r="B163" s="20" t="s">
         <v>24</v>
@@ -10040,7 +10010,7 @@
       </c>
       <c r="I163" s="20"/>
     </row>
-    <row r="164" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:9" ht="15">
       <c r="A164" s="20"/>
       <c r="B164" s="20" t="s">
         <v>24</v>
@@ -10063,7 +10033,7 @@
       </c>
       <c r="I164" s="20"/>
     </row>
-    <row r="165" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:9" ht="15">
       <c r="A165" s="20"/>
       <c r="B165" s="20" t="s">
         <v>24</v>
@@ -10086,7 +10056,7 @@
       </c>
       <c r="I165" s="20"/>
     </row>
-    <row r="166" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:9" ht="15">
       <c r="A166" s="20"/>
       <c r="B166" s="20" t="s">
         <v>24</v>
@@ -10109,7 +10079,7 @@
       </c>
       <c r="I166" s="20"/>
     </row>
-    <row r="167" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:9" ht="15">
       <c r="A167" s="20" t="b">
         <v>0</v>
       </c>
@@ -10128,7 +10098,7 @@
       <c r="H167" s="20"/>
       <c r="I167" s="20"/>
     </row>
-    <row r="168" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:9" ht="15">
       <c r="A168" s="20"/>
       <c r="B168" s="20" t="s">
         <v>24</v>
@@ -10153,7 +10123,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="169" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:9" ht="15">
       <c r="A169" s="20"/>
       <c r="B169" s="20" t="s">
         <v>24</v>
@@ -10176,7 +10146,7 @@
       </c>
       <c r="I169" s="20"/>
     </row>
-    <row r="170" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:9" ht="15">
       <c r="A170" s="20"/>
       <c r="B170" s="20" t="s">
         <v>24</v>
@@ -10199,7 +10169,7 @@
       </c>
       <c r="I170" s="20"/>
     </row>
-    <row r="171" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:9" ht="15">
       <c r="A171" s="20"/>
       <c r="B171" s="20" t="s">
         <v>24</v>
@@ -10222,7 +10192,7 @@
       </c>
       <c r="I171" s="20"/>
     </row>
-    <row r="172" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:9" ht="15">
       <c r="A172" s="20"/>
       <c r="B172" s="20" t="s">
         <v>24</v>
@@ -10245,7 +10215,7 @@
       </c>
       <c r="I172" s="20"/>
     </row>
-    <row r="173" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:9" ht="15">
       <c r="A173" s="20"/>
       <c r="B173" s="20" t="s">
         <v>24</v>
@@ -10268,7 +10238,7 @@
       </c>
       <c r="I173" s="20"/>
     </row>
-    <row r="174" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:9" ht="15">
       <c r="A174" s="20"/>
       <c r="B174" s="20" t="s">
         <v>24</v>
@@ -10291,7 +10261,7 @@
       </c>
       <c r="I174" s="20"/>
     </row>
-    <row r="175" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:9" ht="15">
       <c r="A175" s="20"/>
       <c r="B175" s="20" t="s">
         <v>24</v>
@@ -10314,7 +10284,7 @@
       </c>
       <c r="I175" s="20"/>
     </row>
-    <row r="176" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:9" ht="15">
       <c r="A176" s="20"/>
       <c r="B176" s="20" t="s">
         <v>24</v>
@@ -10337,7 +10307,7 @@
       </c>
       <c r="I176" s="20"/>
     </row>
-    <row r="177" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:9" ht="15">
       <c r="A177" s="20"/>
       <c r="B177" s="20" t="s">
         <v>24</v>
@@ -10360,7 +10330,7 @@
       </c>
       <c r="I177" s="20"/>
     </row>
-    <row r="178" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:9" ht="15">
       <c r="A178" s="20" t="b">
         <v>0</v>
       </c>
@@ -10379,7 +10349,7 @@
       <c r="H178" s="20"/>
       <c r="I178" s="20"/>
     </row>
-    <row r="179" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:9" ht="15">
       <c r="A179" s="20"/>
       <c r="B179" s="20" t="s">
         <v>24</v>
@@ -10402,7 +10372,7 @@
       </c>
       <c r="I179" s="20"/>
     </row>
-    <row r="180" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:9" ht="15">
       <c r="A180" s="20"/>
       <c r="B180" s="20" t="s">
         <v>24</v>
@@ -10425,7 +10395,7 @@
       </c>
       <c r="I180" s="20"/>
     </row>
-    <row r="181" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:9" ht="15">
       <c r="A181" s="20"/>
       <c r="B181" s="20" t="s">
         <v>24</v>
@@ -10448,7 +10418,7 @@
       </c>
       <c r="I181" s="20"/>
     </row>
-    <row r="182" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:9" ht="15">
       <c r="A182" s="20"/>
       <c r="B182" s="20" t="s">
         <v>24</v>
@@ -10471,7 +10441,7 @@
       </c>
       <c r="I182" s="20"/>
     </row>
-    <row r="183" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:9" ht="15">
       <c r="A183" s="20" t="b">
         <v>0</v>
       </c>
@@ -10490,7 +10460,7 @@
       <c r="H183" s="20"/>
       <c r="I183" s="20"/>
     </row>
-    <row r="184" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:9" ht="15">
       <c r="A184" s="20"/>
       <c r="B184" s="20" t="s">
         <v>24</v>
@@ -10513,7 +10483,7 @@
       </c>
       <c r="I184" s="20"/>
     </row>
-    <row r="185" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:9" ht="15">
       <c r="A185" s="20"/>
       <c r="B185" s="20" t="s">
         <v>24</v>
@@ -10536,7 +10506,7 @@
       </c>
       <c r="I185" s="20"/>
     </row>
-    <row r="186" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:9" ht="15">
       <c r="A186" s="20"/>
       <c r="B186" s="20" t="s">
         <v>24</v>
@@ -10559,7 +10529,7 @@
       </c>
       <c r="I186" s="20"/>
     </row>
-    <row r="187" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:9" ht="15">
       <c r="A187" s="20"/>
       <c r="B187" s="20" t="s">
         <v>24</v>
@@ -10582,7 +10552,7 @@
       </c>
       <c r="I187" s="20"/>
     </row>
-    <row r="188" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:9" ht="15">
       <c r="A188" s="20" t="b">
         <v>0</v>
       </c>
@@ -10601,7 +10571,7 @@
       <c r="H188" s="20"/>
       <c r="I188" s="20"/>
     </row>
-    <row r="189" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:9" ht="15">
       <c r="A189" s="20"/>
       <c r="B189" s="20" t="s">
         <v>24</v>
@@ -10622,7 +10592,7 @@
       <c r="H189" s="20"/>
       <c r="I189" s="20"/>
     </row>
-    <row r="190" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:9" ht="15">
       <c r="A190" s="20"/>
       <c r="B190" s="20" t="s">
         <v>24</v>
@@ -10645,7 +10615,7 @@
       </c>
       <c r="I190" s="20"/>
     </row>
-    <row r="191" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:9" ht="15">
       <c r="A191" s="20" t="b">
         <v>0</v>
       </c>
@@ -10664,7 +10634,7 @@
       <c r="H191" s="20"/>
       <c r="I191" s="20"/>
     </row>
-    <row r="192" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:9" ht="15">
       <c r="A192" s="20"/>
       <c r="B192" s="20" t="s">
         <v>24</v>
@@ -10687,7 +10657,7 @@
       </c>
       <c r="I192" s="20"/>
     </row>
-    <row r="193" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:9" ht="15">
       <c r="A193" s="20"/>
       <c r="B193" s="20" t="s">
         <v>24</v>
@@ -10712,7 +10682,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="194" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:9" ht="15">
       <c r="A194" s="20"/>
       <c r="B194" s="20" t="s">
         <v>24</v>
@@ -10733,7 +10703,7 @@
       <c r="H194" s="20"/>
       <c r="I194" s="20"/>
     </row>
-    <row r="195" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:9" ht="15">
       <c r="A195" s="20"/>
       <c r="B195" s="20" t="s">
         <v>24</v>
@@ -10758,7 +10728,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="196" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:9" ht="15">
       <c r="A196" s="20"/>
       <c r="B196" s="20" t="s">
         <v>24</v>
@@ -10783,7 +10753,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="197" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:9" ht="15">
       <c r="A197" s="20" t="b">
         <v>0</v>
       </c>
@@ -10802,7 +10772,7 @@
       <c r="H197" s="20"/>
       <c r="I197" s="20"/>
     </row>
-    <row r="198" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:9" ht="15">
       <c r="A198" s="20"/>
       <c r="B198" s="20" t="s">
         <v>24</v>
@@ -10827,7 +10797,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="199" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:9" ht="15">
       <c r="A199" s="20"/>
       <c r="B199" s="20" t="s">
         <v>24</v>
@@ -10850,7 +10820,7 @@
       </c>
       <c r="I199" s="20"/>
     </row>
-    <row r="200" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:9" ht="15">
       <c r="A200" s="20"/>
       <c r="B200" s="20" t="s">
         <v>24</v>
@@ -10873,7 +10843,7 @@
       </c>
       <c r="I200" s="20"/>
     </row>
-    <row r="201" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:9" ht="15">
       <c r="A201" s="20"/>
       <c r="B201" s="20" t="s">
         <v>24</v>
@@ -10896,7 +10866,7 @@
       </c>
       <c r="I201" s="20"/>
     </row>
-    <row r="202" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:9" ht="15">
       <c r="A202" s="20"/>
       <c r="B202" s="20" t="s">
         <v>24</v>
@@ -10919,7 +10889,7 @@
       </c>
       <c r="I202" s="20"/>
     </row>
-    <row r="203" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:9" ht="15">
       <c r="A203" s="20"/>
       <c r="B203" s="20" t="s">
         <v>24</v>
@@ -10942,7 +10912,7 @@
       </c>
       <c r="I203" s="20"/>
     </row>
-    <row r="204" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:9" ht="15">
       <c r="A204" s="20"/>
       <c r="B204" s="20" t="s">
         <v>24</v>
@@ -10965,7 +10935,7 @@
       </c>
       <c r="I204" s="20"/>
     </row>
-    <row r="205" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:9" ht="15">
       <c r="A205" s="20"/>
       <c r="B205" s="20" t="s">
         <v>24</v>
@@ -10988,7 +10958,7 @@
       </c>
       <c r="I205" s="20"/>
     </row>
-    <row r="206" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:9" ht="15">
       <c r="A206" s="20"/>
       <c r="B206" s="20" t="s">
         <v>24</v>
@@ -11011,7 +10981,7 @@
       </c>
       <c r="I206" s="20"/>
     </row>
-    <row r="207" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:9" ht="15">
       <c r="A207" s="20" t="b">
         <v>0</v>
       </c>
@@ -11030,7 +11000,7 @@
       <c r="H207" s="20"/>
       <c r="I207" s="20"/>
     </row>
-    <row r="208" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:9" ht="15">
       <c r="A208" s="20"/>
       <c r="B208" s="20" t="s">
         <v>24</v>
@@ -11055,7 +11025,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="209" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:9" ht="15">
       <c r="A209" s="20"/>
       <c r="B209" s="20" t="s">
         <v>24</v>
@@ -11078,7 +11048,7 @@
       </c>
       <c r="I209" s="20"/>
     </row>
-    <row r="210" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:9" ht="15">
       <c r="A210" s="20"/>
       <c r="B210" s="20" t="s">
         <v>24</v>
@@ -11101,7 +11071,7 @@
       </c>
       <c r="I210" s="20"/>
     </row>
-    <row r="211" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:9" ht="15">
       <c r="A211" s="20"/>
       <c r="B211" s="20" t="s">
         <v>24</v>
@@ -11124,7 +11094,7 @@
       </c>
       <c r="I211" s="20"/>
     </row>
-    <row r="212" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:9" ht="15">
       <c r="A212" s="20"/>
       <c r="B212" s="20" t="s">
         <v>24</v>
@@ -11147,7 +11117,7 @@
       </c>
       <c r="I212" s="20"/>
     </row>
-    <row r="213" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:9" ht="15">
       <c r="A213" s="20"/>
       <c r="B213" s="20" t="s">
         <v>24</v>
@@ -11170,7 +11140,7 @@
       </c>
       <c r="I213" s="20"/>
     </row>
-    <row r="214" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:9" ht="15">
       <c r="A214" s="20"/>
       <c r="B214" s="20" t="s">
         <v>24</v>
@@ -11193,7 +11163,7 @@
       </c>
       <c r="I214" s="20"/>
     </row>
-    <row r="215" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:9" ht="15">
       <c r="A215" s="20"/>
       <c r="B215" s="20" t="s">
         <v>24</v>
@@ -11216,7 +11186,7 @@
       </c>
       <c r="I215" s="20"/>
     </row>
-    <row r="216" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:9" ht="15">
       <c r="A216" s="20"/>
       <c r="B216" s="20" t="s">
         <v>24</v>
@@ -11239,7 +11209,7 @@
       </c>
       <c r="I216" s="20"/>
     </row>
-    <row r="217" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:9" ht="15">
       <c r="A217" s="20" t="b">
         <v>0</v>
       </c>
@@ -11258,7 +11228,7 @@
       <c r="H217" s="20"/>
       <c r="I217" s="20"/>
     </row>
-    <row r="218" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:9" ht="15">
       <c r="A218" s="20"/>
       <c r="B218" s="20" t="s">
         <v>24</v>
@@ -11279,7 +11249,7 @@
       <c r="H218" s="20"/>
       <c r="I218" s="20"/>
     </row>
-    <row r="219" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:9" ht="15">
       <c r="A219" s="20"/>
       <c r="B219" s="20" t="s">
         <v>24</v>
@@ -11302,7 +11272,7 @@
       </c>
       <c r="I219" s="20"/>
     </row>
-    <row r="220" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:9" ht="15">
       <c r="A220" s="20"/>
       <c r="B220" s="20" t="s">
         <v>24</v>
@@ -11325,7 +11295,7 @@
       </c>
       <c r="I220" s="20"/>
     </row>
-    <row r="221" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:9" ht="15">
       <c r="A221" s="20"/>
       <c r="B221" s="20" t="s">
         <v>24</v>
@@ -11348,7 +11318,7 @@
       </c>
       <c r="I221" s="20"/>
     </row>
-    <row r="222" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:9" ht="15">
       <c r="A222" s="20"/>
       <c r="B222" s="20" t="s">
         <v>24</v>
@@ -11371,7 +11341,7 @@
       </c>
       <c r="I222" s="20"/>
     </row>
-    <row r="223" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:9" ht="15">
       <c r="A223" s="20"/>
       <c r="B223" s="20" t="s">
         <v>24</v>
@@ -11394,7 +11364,7 @@
       </c>
       <c r="I223" s="20"/>
     </row>
-    <row r="224" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:9" ht="15">
       <c r="A224" s="20"/>
       <c r="B224" s="20" t="s">
         <v>24</v>
@@ -11417,7 +11387,7 @@
       </c>
       <c r="I224" s="20"/>
     </row>
-    <row r="225" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:9" ht="15">
       <c r="A225" s="20"/>
       <c r="B225" s="20" t="s">
         <v>24</v>
@@ -11440,7 +11410,7 @@
       </c>
       <c r="I225" s="20"/>
     </row>
-    <row r="226" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:9" ht="15">
       <c r="A226" s="20"/>
       <c r="B226" s="20" t="s">
         <v>24</v>
@@ -11463,7 +11433,7 @@
       </c>
       <c r="I226" s="20"/>
     </row>
-    <row r="227" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:9" ht="15">
       <c r="A227" s="20"/>
       <c r="B227" s="20" t="s">
         <v>24</v>
@@ -11486,7 +11456,7 @@
       </c>
       <c r="I227" s="20"/>
     </row>
-    <row r="228" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:9" ht="15">
       <c r="A228" s="20"/>
       <c r="B228" s="20" t="s">
         <v>24</v>
@@ -11509,7 +11479,7 @@
       </c>
       <c r="I228" s="20"/>
     </row>
-    <row r="229" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:9" ht="15">
       <c r="A229" s="20"/>
       <c r="B229" s="20" t="s">
         <v>24</v>
@@ -11532,7 +11502,7 @@
       </c>
       <c r="I229" s="20"/>
     </row>
-    <row r="230" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:9" ht="15">
       <c r="A230" s="20"/>
       <c r="B230" s="20" t="s">
         <v>24</v>
@@ -11555,7 +11525,7 @@
       </c>
       <c r="I230" s="20"/>
     </row>
-    <row r="231" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:9" ht="15">
       <c r="A231" s="20"/>
       <c r="B231" s="20" t="s">
         <v>24</v>
@@ -11578,7 +11548,7 @@
       </c>
       <c r="I231" s="20"/>
     </row>
-    <row r="232" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:9" ht="15">
       <c r="A232" s="20"/>
       <c r="B232" s="20" t="s">
         <v>24</v>
@@ -11601,7 +11571,7 @@
       </c>
       <c r="I232" s="20"/>
     </row>
-    <row r="233" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:9" ht="15">
       <c r="A233" s="20"/>
       <c r="B233" s="20" t="s">
         <v>24</v>
@@ -11624,7 +11594,7 @@
       </c>
       <c r="I233" s="20"/>
     </row>
-    <row r="234" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:9" ht="15">
       <c r="A234" s="20" t="b">
         <v>0</v>
       </c>
@@ -11643,7 +11613,7 @@
       <c r="H234" s="20"/>
       <c r="I234" s="20"/>
     </row>
-    <row r="235" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:9" ht="15">
       <c r="A235" s="20"/>
       <c r="B235" s="20" t="s">
         <v>24</v>
@@ -11664,7 +11634,7 @@
       <c r="H235" s="20"/>
       <c r="I235" s="20"/>
     </row>
-    <row r="236" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:9" ht="15">
       <c r="A236" s="20"/>
       <c r="B236" s="20" t="s">
         <v>24</v>
@@ -11687,7 +11657,7 @@
       </c>
       <c r="I236" s="20"/>
     </row>
-    <row r="237" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:9" ht="15">
       <c r="A237" s="20"/>
       <c r="B237" s="20" t="s">
         <v>24</v>
@@ -11710,7 +11680,7 @@
       </c>
       <c r="I237" s="20"/>
     </row>
-    <row r="238" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:9" ht="15">
       <c r="A238" s="20"/>
       <c r="B238" s="20" t="s">
         <v>24</v>
@@ -11733,7 +11703,7 @@
       </c>
       <c r="I238" s="20"/>
     </row>
-    <row r="239" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:9" ht="15">
       <c r="A239" s="20"/>
       <c r="B239" s="20" t="s">
         <v>24</v>
@@ -11756,7 +11726,7 @@
       </c>
       <c r="I239" s="20"/>
     </row>
-    <row r="240" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:9" ht="15">
       <c r="A240" s="20"/>
       <c r="B240" s="20" t="s">
         <v>24</v>
@@ -11779,7 +11749,7 @@
       </c>
       <c r="I240" s="20"/>
     </row>
-    <row r="241" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:9" ht="15">
       <c r="A241" s="20"/>
       <c r="B241" s="20" t="s">
         <v>24</v>
@@ -11802,7 +11772,7 @@
       </c>
       <c r="I241" s="20"/>
     </row>
-    <row r="242" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:9" ht="15">
       <c r="A242" s="20"/>
       <c r="B242" s="20" t="s">
         <v>24</v>
@@ -11825,7 +11795,7 @@
       </c>
       <c r="I242" s="20"/>
     </row>
-    <row r="243" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:9" ht="15">
       <c r="A243" s="20"/>
       <c r="B243" s="20" t="s">
         <v>24</v>
@@ -11848,7 +11818,7 @@
       </c>
       <c r="I243" s="20"/>
     </row>
-    <row r="244" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:9" ht="15">
       <c r="A244" s="20"/>
       <c r="B244" s="20" t="s">
         <v>24</v>
@@ -11871,7 +11841,7 @@
       </c>
       <c r="I244" s="20"/>
     </row>
-    <row r="245" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:9" ht="15">
       <c r="A245" s="20"/>
       <c r="B245" s="20" t="s">
         <v>24</v>
@@ -11894,7 +11864,7 @@
       </c>
       <c r="I245" s="20"/>
     </row>
-    <row r="246" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:9" ht="15">
       <c r="A246" s="20"/>
       <c r="B246" s="20" t="s">
         <v>24</v>
@@ -11917,7 +11887,7 @@
       </c>
       <c r="I246" s="20"/>
     </row>
-    <row r="247" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:9" ht="15">
       <c r="A247" s="20"/>
       <c r="B247" s="20" t="s">
         <v>24</v>
@@ -11940,7 +11910,7 @@
       </c>
       <c r="I247" s="20"/>
     </row>
-    <row r="248" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:9" ht="15">
       <c r="A248" s="20"/>
       <c r="B248" s="20" t="s">
         <v>24</v>
@@ -11963,7 +11933,7 @@
       </c>
       <c r="I248" s="20"/>
     </row>
-    <row r="249" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:9" ht="15">
       <c r="A249" s="20"/>
       <c r="B249" s="20" t="s">
         <v>24</v>
@@ -11986,7 +11956,7 @@
       </c>
       <c r="I249" s="20"/>
     </row>
-    <row r="250" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:9" ht="15">
       <c r="A250" s="20"/>
       <c r="B250" s="20" t="s">
         <v>24</v>
@@ -12009,7 +11979,7 @@
       </c>
       <c r="I250" s="20"/>
     </row>
-    <row r="251" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:9" ht="15">
       <c r="A251" s="20" t="b">
         <v>0</v>
       </c>
@@ -12028,7 +11998,7 @@
       <c r="H251" s="20"/>
       <c r="I251" s="20"/>
     </row>
-    <row r="252" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:9" ht="15">
       <c r="A252" s="20"/>
       <c r="B252" s="20" t="s">
         <v>24</v>
@@ -12053,7 +12023,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="253" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:9" ht="15">
       <c r="A253" s="20"/>
       <c r="B253" s="20" t="s">
         <v>24</v>
@@ -12076,7 +12046,7 @@
       </c>
       <c r="I253" s="20"/>
     </row>
-    <row r="254" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:9" ht="15">
       <c r="A254" s="20"/>
       <c r="B254" s="20" t="s">
         <v>24</v>
@@ -12099,7 +12069,7 @@
       </c>
       <c r="I254" s="20"/>
     </row>
-    <row r="255" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:9" ht="15">
       <c r="A255" s="20"/>
       <c r="B255" s="20" t="s">
         <v>24</v>
@@ -12122,7 +12092,7 @@
       </c>
       <c r="I255" s="20"/>
     </row>
-    <row r="256" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:9" ht="15">
       <c r="A256" s="20"/>
       <c r="B256" s="20" t="s">
         <v>24</v>
@@ -12145,7 +12115,7 @@
       </c>
       <c r="I256" s="20"/>
     </row>
-    <row r="257" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:9" ht="15">
       <c r="A257" s="20" t="b">
         <v>0</v>
       </c>
@@ -12164,7 +12134,7 @@
       <c r="H257" s="20"/>
       <c r="I257" s="20"/>
     </row>
-    <row r="258" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:9" ht="15">
       <c r="A258" s="20"/>
       <c r="B258" s="20" t="s">
         <v>24</v>
@@ -12189,7 +12159,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="259" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:9" ht="15">
       <c r="A259" s="20"/>
       <c r="B259" s="20" t="s">
         <v>24</v>
@@ -12212,7 +12182,7 @@
       </c>
       <c r="I259" s="20"/>
     </row>
-    <row r="260" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:9" ht="15">
       <c r="A260" s="20" t="b">
         <v>0</v>
       </c>
@@ -12231,7 +12201,7 @@
       <c r="H260" s="20"/>
       <c r="I260" s="20"/>
     </row>
-    <row r="261" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:9" ht="15">
       <c r="A261" s="20" t="b">
         <v>0</v>
       </c>
@@ -12250,7 +12220,7 @@
       <c r="H261" s="20"/>
       <c r="I261" s="20"/>
     </row>
-    <row r="262" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:9" ht="15">
       <c r="A262" s="20" t="b">
         <v>0</v>
       </c>
@@ -12269,7 +12239,7 @@
       <c r="H262" s="20"/>
       <c r="I262" s="20"/>
     </row>
-    <row r="263" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:9" ht="15">
       <c r="A263" s="20"/>
       <c r="B263" s="20" t="s">
         <v>24</v>
@@ -12290,7 +12260,7 @@
       <c r="H263" s="20"/>
       <c r="I263" s="20"/>
     </row>
-    <row r="264" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:9" ht="15">
       <c r="A264" s="20"/>
       <c r="B264" s="20" t="s">
         <v>24</v>
@@ -12313,7 +12283,7 @@
       </c>
       <c r="I264" s="20"/>
     </row>
-    <row r="265" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:9" ht="15">
       <c r="A265" s="20"/>
       <c r="B265" s="20" t="s">
         <v>24</v>
@@ -12336,7 +12306,7 @@
       </c>
       <c r="I265" s="20"/>
     </row>
-    <row r="266" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:9" ht="15">
       <c r="A266" s="20"/>
       <c r="B266" s="20" t="s">
         <v>24</v>
@@ -12359,7 +12329,7 @@
       </c>
       <c r="I266" s="20"/>
     </row>
-    <row r="267" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:9" ht="15">
       <c r="A267" s="20"/>
       <c r="B267" s="20" t="s">
         <v>24</v>
@@ -12382,7 +12352,7 @@
       </c>
       <c r="I267" s="20"/>
     </row>
-    <row r="268" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:9" ht="15">
       <c r="A268" s="20"/>
       <c r="B268" s="20" t="s">
         <v>24</v>
@@ -12405,7 +12375,7 @@
       </c>
       <c r="I268" s="20"/>
     </row>
-    <row r="269" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:9" ht="15">
       <c r="A269" s="20"/>
       <c r="B269" s="20" t="s">
         <v>24</v>
@@ -12428,7 +12398,7 @@
       </c>
       <c r="I269" s="20"/>
     </row>
-    <row r="270" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:9" ht="15">
       <c r="A270" s="20"/>
       <c r="B270" s="20" t="s">
         <v>24</v>
@@ -12451,7 +12421,7 @@
       </c>
       <c r="I270" s="20"/>
     </row>
-    <row r="271" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:9" ht="15">
       <c r="A271" s="20"/>
       <c r="B271" s="20" t="s">
         <v>24</v>
@@ -12474,7 +12444,7 @@
       </c>
       <c r="I271" s="20"/>
     </row>
-    <row r="272" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:9" ht="15">
       <c r="A272" s="20"/>
       <c r="B272" s="20" t="s">
         <v>24</v>
@@ -12497,7 +12467,7 @@
       </c>
       <c r="I272" s="20"/>
     </row>
-    <row r="273" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:9" ht="15">
       <c r="A273" s="20"/>
       <c r="B273" s="20" t="s">
         <v>24</v>
@@ -12520,7 +12490,7 @@
       </c>
       <c r="I273" s="20"/>
     </row>
-    <row r="274" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:9" ht="15">
       <c r="A274" s="20" t="b">
         <v>0</v>
       </c>
@@ -12539,7 +12509,7 @@
       <c r="H274" s="20"/>
       <c r="I274" s="20"/>
     </row>
-    <row r="275" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:9" ht="15">
       <c r="A275" s="20"/>
       <c r="B275" s="20" t="s">
         <v>24</v>
@@ -12562,7 +12532,7 @@
       </c>
       <c r="I275" s="20"/>
     </row>
-    <row r="276" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:9" ht="15">
       <c r="A276" s="20" t="b">
         <v>0</v>
       </c>
@@ -12581,7 +12551,7 @@
       <c r="H276" s="20"/>
       <c r="I276" s="20"/>
     </row>
-    <row r="277" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:9" ht="15">
       <c r="A277" s="20"/>
       <c r="B277" s="20" t="s">
         <v>24</v>
@@ -12606,7 +12576,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="278" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:9" ht="15">
       <c r="A278" s="20"/>
       <c r="B278" s="20" t="s">
         <v>24</v>
@@ -12629,7 +12599,7 @@
       </c>
       <c r="I278" s="20"/>
     </row>
-    <row r="279" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:9" ht="15">
       <c r="A279" s="20"/>
       <c r="B279" s="20" t="s">
         <v>24</v>
@@ -12652,7 +12622,7 @@
       </c>
       <c r="I279" s="20"/>
     </row>
-    <row r="280" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:9" ht="15">
       <c r="A280" s="20"/>
       <c r="B280" s="20" t="s">
         <v>24</v>
@@ -12675,7 +12645,7 @@
       </c>
       <c r="I280" s="20"/>
     </row>
-    <row r="281" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:9" ht="15">
       <c r="A281" s="20"/>
       <c r="B281" s="20" t="s">
         <v>24</v>
@@ -12698,7 +12668,7 @@
       </c>
       <c r="I281" s="20"/>
     </row>
-    <row r="282" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:9" ht="15">
       <c r="A282" s="20"/>
       <c r="B282" s="20" t="s">
         <v>24</v>
@@ -12721,7 +12691,7 @@
       </c>
       <c r="I282" s="20"/>
     </row>
-    <row r="283" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:9" ht="15">
       <c r="A283" s="20"/>
       <c r="B283" s="20" t="s">
         <v>24</v>
@@ -12744,7 +12714,7 @@
       </c>
       <c r="I283" s="20"/>
     </row>
-    <row r="284" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:9" ht="15">
       <c r="A284" s="20"/>
       <c r="B284" s="20" t="s">
         <v>24</v>
@@ -12767,7 +12737,7 @@
       </c>
       <c r="I284" s="20"/>
     </row>
-    <row r="285" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:9" ht="15">
       <c r="A285" s="20"/>
       <c r="B285" s="20" t="s">
         <v>24</v>
@@ -12790,7 +12760,7 @@
       </c>
       <c r="I285" s="20"/>
     </row>
-    <row r="286" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:9" ht="15">
       <c r="A286" s="20"/>
       <c r="B286" s="20" t="s">
         <v>24</v>
@@ -12813,7 +12783,7 @@
       </c>
       <c r="I286" s="20"/>
     </row>
-    <row r="287" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:9" ht="15">
       <c r="A287" s="20"/>
       <c r="B287" s="20" t="s">
         <v>24</v>
@@ -12836,7 +12806,7 @@
       </c>
       <c r="I287" s="20"/>
     </row>
-    <row r="288" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:9" ht="15">
       <c r="A288" s="20" t="b">
         <v>0</v>
       </c>
@@ -12855,7 +12825,7 @@
       <c r="H288" s="20"/>
       <c r="I288" s="20"/>
     </row>
-    <row r="289" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:9" ht="15">
       <c r="A289" s="20"/>
       <c r="B289" s="20" t="s">
         <v>24</v>
@@ -12878,7 +12848,7 @@
       </c>
       <c r="I289" s="20"/>
     </row>
-    <row r="290" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:9" ht="15">
       <c r="A290" s="20" t="b">
         <v>0</v>
       </c>
@@ -12897,7 +12867,7 @@
       <c r="H290" s="20"/>
       <c r="I290" s="20"/>
     </row>
-    <row r="291" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:9" ht="15">
       <c r="A291" s="20"/>
       <c r="B291" s="20" t="s">
         <v>24</v>
@@ -12918,7 +12888,7 @@
       <c r="H291" s="20"/>
       <c r="I291" s="20"/>
     </row>
-    <row r="292" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:9" ht="15">
       <c r="A292" s="20" t="b">
         <v>0</v>
       </c>
@@ -12937,7 +12907,7 @@
       <c r="H292" s="20"/>
       <c r="I292" s="20"/>
     </row>
-    <row r="293" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:9" ht="15">
       <c r="A293" s="20"/>
       <c r="B293" s="20" t="s">
         <v>24</v>
@@ -12958,7 +12928,7 @@
       <c r="H293" s="20"/>
       <c r="I293" s="20"/>
     </row>
-    <row r="294" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:9" ht="15">
       <c r="A294" s="20" t="b">
         <v>0</v>
       </c>
@@ -12977,7 +12947,7 @@
       <c r="H294" s="20"/>
       <c r="I294" s="20"/>
     </row>
-    <row r="295" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:9" ht="15">
       <c r="A295" s="20"/>
       <c r="B295" s="20" t="s">
         <v>24</v>
@@ -12998,7 +12968,7 @@
       <c r="H295" s="20"/>
       <c r="I295" s="20"/>
     </row>
-    <row r="296" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:9" ht="15">
       <c r="A296" s="20" t="b">
         <v>0</v>
       </c>
@@ -13017,7 +12987,7 @@
       <c r="H296" s="20"/>
       <c r="I296" s="20"/>
     </row>
-    <row r="297" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:9" ht="15">
       <c r="A297" s="20"/>
       <c r="B297" s="20" t="s">
         <v>24</v>
@@ -13040,7 +13010,7 @@
       </c>
       <c r="I297" s="20"/>
     </row>
-    <row r="298" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:9" ht="15">
       <c r="A298" s="20" t="b">
         <v>0</v>
       </c>
@@ -13059,7 +13029,7 @@
       <c r="H298" s="20"/>
       <c r="I298" s="20"/>
     </row>
-    <row r="299" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:9" ht="15">
       <c r="A299" s="20"/>
       <c r="B299" s="20" t="s">
         <v>24</v>
@@ -13084,7 +13054,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="300" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:9" ht="15">
       <c r="A300" s="20"/>
       <c r="B300" s="20" t="s">
         <v>24</v>
@@ -13107,7 +13077,7 @@
       </c>
       <c r="I300" s="20"/>
     </row>
-    <row r="301" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:9" ht="15">
       <c r="A301" s="20"/>
       <c r="B301" s="20" t="s">
         <v>24</v>
@@ -13130,7 +13100,7 @@
       </c>
       <c r="I301" s="20"/>
     </row>
-    <row r="302" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:9" ht="15">
       <c r="A302" s="20"/>
       <c r="B302" s="20" t="s">
         <v>24</v>
@@ -13153,7 +13123,7 @@
       </c>
       <c r="I302" s="20"/>
     </row>
-    <row r="303" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:9" ht="15">
       <c r="A303" s="20"/>
       <c r="B303" s="20" t="s">
         <v>24</v>
@@ -13176,7 +13146,7 @@
       </c>
       <c r="I303" s="20"/>
     </row>
-    <row r="304" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:9" ht="15">
       <c r="A304" s="20"/>
       <c r="B304" s="20" t="s">
         <v>24</v>
@@ -13199,7 +13169,7 @@
       </c>
       <c r="I304" s="20"/>
     </row>
-    <row r="305" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:9" ht="15">
       <c r="A305" s="20"/>
       <c r="B305" s="20" t="s">
         <v>24</v>
@@ -13222,7 +13192,7 @@
       </c>
       <c r="I305" s="20"/>
     </row>
-    <row r="306" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:9" ht="15">
       <c r="A306" s="20"/>
       <c r="B306" s="20" t="s">
         <v>24</v>
@@ -13245,7 +13215,7 @@
       </c>
       <c r="I306" s="20"/>
     </row>
-    <row r="307" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:9" ht="15">
       <c r="A307" s="20"/>
       <c r="B307" s="20" t="s">
         <v>24</v>
@@ -13268,7 +13238,7 @@
       </c>
       <c r="I307" s="20"/>
     </row>
-    <row r="308" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:9" ht="15">
       <c r="A308" s="20" t="b">
         <v>0</v>
       </c>
@@ -13287,7 +13257,7 @@
       <c r="H308" s="20"/>
       <c r="I308" s="20"/>
     </row>
-    <row r="309" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:9" ht="15">
       <c r="A309" s="20"/>
       <c r="B309" s="20" t="s">
         <v>24</v>
@@ -13310,7 +13280,7 @@
       </c>
       <c r="I309" s="20"/>
     </row>
-    <row r="310" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:9" ht="15">
       <c r="A310" s="20"/>
       <c r="B310" s="20" t="s">
         <v>24</v>
@@ -13333,7 +13303,7 @@
       </c>
       <c r="I310" s="20"/>
     </row>
-    <row r="311" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:9" ht="15">
       <c r="A311" s="20"/>
       <c r="B311" s="20" t="s">
         <v>24</v>
@@ -13356,7 +13326,7 @@
       </c>
       <c r="I311" s="20"/>
     </row>
-    <row r="312" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:9" ht="15">
       <c r="A312" s="20"/>
       <c r="B312" s="20" t="s">
         <v>24</v>
@@ -13379,7 +13349,7 @@
       </c>
       <c r="I312" s="20"/>
     </row>
-    <row r="313" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:9" ht="15">
       <c r="A313" s="20" t="b">
         <v>0</v>
       </c>
@@ -13398,7 +13368,7 @@
       <c r="H313" s="20"/>
       <c r="I313" s="20"/>
     </row>
-    <row r="314" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:9" ht="15">
       <c r="A314" s="20"/>
       <c r="B314" s="20" t="s">
         <v>24</v>
@@ -13421,7 +13391,7 @@
       </c>
       <c r="I314" s="20"/>
     </row>
-    <row r="315" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:9" ht="15">
       <c r="A315" s="20"/>
       <c r="B315" s="20" t="s">
         <v>24</v>
@@ -13444,7 +13414,7 @@
       </c>
       <c r="I315" s="20"/>
     </row>
-    <row r="316" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:9" ht="15">
       <c r="A316" s="20"/>
       <c r="B316" s="20" t="s">
         <v>24</v>
@@ -13469,7 +13439,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="317" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:9" ht="15">
       <c r="A317" s="20" t="b">
         <v>0</v>
       </c>
@@ -13488,7 +13458,7 @@
       <c r="H317" s="20"/>
       <c r="I317" s="20"/>
     </row>
-    <row r="318" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:9" ht="15">
       <c r="A318" s="20"/>
       <c r="B318" s="20" t="s">
         <v>24</v>
@@ -13513,7 +13483,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="319" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:9" ht="15">
       <c r="A319" s="20"/>
       <c r="B319" s="20" t="s">
         <v>24</v>
@@ -13536,7 +13506,7 @@
       </c>
       <c r="I319" s="20"/>
     </row>
-    <row r="320" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:9" ht="15">
       <c r="A320" s="20" t="b">
         <v>0</v>
       </c>
@@ -13555,7 +13525,7 @@
       <c r="H320" s="20"/>
       <c r="I320" s="20"/>
     </row>
-    <row r="321" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:9" ht="15">
       <c r="A321" s="20"/>
       <c r="B321" s="20" t="s">
         <v>24</v>
@@ -13576,7 +13546,7 @@
       <c r="H321" s="20"/>
       <c r="I321" s="20"/>
     </row>
-    <row r="322" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:9" ht="15">
       <c r="A322" s="20"/>
       <c r="B322" s="20" t="s">
         <v>24</v>
@@ -13597,7 +13567,7 @@
       <c r="H322" s="20"/>
       <c r="I322" s="20"/>
     </row>
-    <row r="323" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:9" ht="15">
       <c r="A323" s="20"/>
       <c r="B323" s="20" t="s">
         <v>24</v>
@@ -13620,7 +13590,7 @@
       </c>
       <c r="I323" s="20"/>
     </row>
-    <row r="324" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:9" ht="15">
       <c r="A324" s="20" t="b">
         <v>0</v>
       </c>
@@ -13639,7 +13609,7 @@
       <c r="H324" s="20"/>
       <c r="I324" s="20"/>
     </row>
-    <row r="325" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:9" ht="15">
       <c r="A325" s="20" t="b">
         <v>0</v>
       </c>
@@ -13658,7 +13628,7 @@
       <c r="H325" s="20"/>
       <c r="I325" s="20"/>
     </row>
-    <row r="326" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:9" ht="15">
       <c r="A326" s="20"/>
       <c r="B326" s="20" t="s">
         <v>24</v>
@@ -13683,7 +13653,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="327" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:9" ht="15">
       <c r="A327" s="20"/>
       <c r="B327" s="20" t="s">
         <v>24</v>

</xml_diff>